<commit_message>
fuzzylogic arithmetic exception no fix
</commit_message>
<xml_diff>
--- a/assets/excel/Minigames.xlsx
+++ b/assets/excel/Minigames.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1-SCHOOL\1-Prog\CodexLearning\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8430AAEF-F062-49CA-ACA6-954970802CC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF20FF8-1B46-4B66-9A89-BEFA64FBEF53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2F4D6A40-7D2F-4386-B1F7-728101A5D7AD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{2F4D6A40-7D2F-4386-B1F7-728101A5D7AD}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeRiddle" sheetId="4" r:id="rId1"/>
@@ -4694,8 +4694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54F442EA-7F5D-4748-9754-A2DC9FAD38BA}">
   <dimension ref="A1:R197"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22989,7 +22989,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F99139-151D-46A7-9406-2704D1F454D5}">
   <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+    <sheetView topLeftCell="A134" workbookViewId="0">
       <selection activeCell="G191" sqref="G191"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
kunin mo lang questionnaire
</commit_message>
<xml_diff>
--- a/assets/excel/Minigames.xlsx
+++ b/assets/excel/Minigames.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ryoshu\Documents\GitHub\CodexLearning2\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D44A92-0C95-49C7-8B74-87EBB2335FB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104852B7-E979-4282-9B51-30415202D665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6615" yWindow="510" windowWidth="12765" windowHeight="12630" activeTab="2" xr2:uid="{2F4D6A40-7D2F-4386-B1F7-728101A5D7AD}"/>
+    <workbookView xWindow="15915" yWindow="735" windowWidth="12765" windowHeight="12630" activeTab="2" xr2:uid="{2F4D6A40-7D2F-4386-B1F7-728101A5D7AD}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeRiddle" sheetId="4" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5051" uniqueCount="1365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5071" uniqueCount="1374">
   <si>
     <t>Stage 1</t>
   </si>
@@ -4835,6 +4835,33 @@
   <si>
     <t>ClassObject()</t>
   </si>
+  <si>
+    <t>/*/</t>
+  </si>
+  <si>
+    <t>\**\</t>
+  </si>
+  <si>
+    <t>\/</t>
+  </si>
+  <si>
+    <t>\\\</t>
+  </si>
+  <si>
+    <t>/\</t>
+  </si>
+  <si>
+    <t>\\ this is a comment</t>
+  </si>
+  <si>
+    <t>\* this is for blocks *\</t>
+  </si>
+  <si>
+    <t>'' documentation '''</t>
+  </si>
+  <si>
+    <t>// this comment</t>
+  </si>
 </sst>
 </file>
 
@@ -4843,7 +4870,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4853,6 +4880,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4875,10 +4910,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4886,8 +4922,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -22859,10 +22897,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6F99139-151D-46A7-9406-2704D1F454D5}">
-  <dimension ref="A1:D201"/>
+  <dimension ref="A1:D211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="D147" sqref="D147"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -23171,13 +23209,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>1255</v>
+        <v>1365</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -23185,13 +23223,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>1256</v>
+        <v>267</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -23199,13 +23237,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>1257</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -23213,13 +23251,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="D25" t="s">
-        <v>1260</v>
+      <c r="D25" s="7" t="s">
+        <v>1368</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -23227,13 +23265,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>1258</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -23241,13 +23279,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C27">
         <v>1</v>
       </c>
       <c r="D27" t="s">
-        <v>1259</v>
+        <v>1369</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -23255,13 +23293,13 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C28">
         <v>1</v>
       </c>
       <c r="D28" t="s">
-        <v>1261</v>
+        <v>1370</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -23269,13 +23307,13 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C29">
         <v>1</v>
       </c>
       <c r="D29" t="s">
-        <v>1262</v>
+        <v>1371</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -23283,13 +23321,13 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C30">
         <v>1</v>
       </c>
-      <c r="D30" t="s">
-        <v>1312</v>
+      <c r="D30" s="3" t="s">
+        <v>1372</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -23297,13 +23335,13 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
       <c r="D31" t="s">
-        <v>1313</v>
+        <v>1373</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -23317,7 +23355,7 @@
         <v>1</v>
       </c>
       <c r="D32" t="s">
-        <v>1314</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -23330,6 +23368,9 @@
       <c r="C33">
         <v>1</v>
       </c>
+      <c r="D33" t="s">
+        <v>1256</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34">
@@ -23341,6 +23382,9 @@
       <c r="C34">
         <v>1</v>
       </c>
+      <c r="D34" t="s">
+        <v>1257</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35">
@@ -23352,6 +23396,9 @@
       <c r="C35">
         <v>1</v>
       </c>
+      <c r="D35" t="s">
+        <v>1260</v>
+      </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36">
@@ -23363,19 +23410,22 @@
       <c r="C36">
         <v>1</v>
       </c>
+      <c r="D36" t="s">
+        <v>1258</v>
+      </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C37">
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>189</v>
+        <v>1259</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -23383,13 +23433,13 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>1159</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -23397,13 +23447,13 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C39">
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>1160</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -23411,13 +23461,13 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C40">
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>1161</v>
+        <v>1312</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -23425,13 +23475,13 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C41">
         <v>1</v>
       </c>
       <c r="D41" t="s">
-        <v>92</v>
+        <v>1313</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -23439,13 +23489,13 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C42">
         <v>1</v>
       </c>
       <c r="D42" t="s">
-        <v>1162</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -23453,13 +23503,10 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C43">
         <v>1</v>
-      </c>
-      <c r="D43" t="s">
-        <v>1163</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -23467,13 +23514,10 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C44">
         <v>1</v>
-      </c>
-      <c r="D44" t="s">
-        <v>1164</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -23481,13 +23525,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C45">
         <v>1</v>
-      </c>
-      <c r="D45" t="s">
-        <v>1165</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -23495,13 +23536,10 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C46">
         <v>1</v>
-      </c>
-      <c r="D46" s="6" t="s">
-        <v>1315</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -23515,7 +23553,7 @@
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>1316</v>
+        <v>189</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -23529,7 +23567,7 @@
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>1317</v>
+        <v>1159</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -23543,7 +23581,7 @@
         <v>1</v>
       </c>
       <c r="D49" t="s">
-        <v>1318</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -23557,7 +23595,7 @@
         <v>1</v>
       </c>
       <c r="D50" t="s">
-        <v>1319</v>
+        <v>1161</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -23571,7 +23609,7 @@
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>1320</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -23579,13 +23617,13 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C52">
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>1263</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -23593,13 +23631,13 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C53">
         <v>1</v>
       </c>
       <c r="D53" t="s">
-        <v>1321</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -23607,13 +23645,13 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C54">
         <v>1</v>
       </c>
       <c r="D54" t="s">
-        <v>1322</v>
+        <v>1164</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -23621,13 +23659,13 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C55">
         <v>1</v>
       </c>
       <c r="D55" t="s">
-        <v>1323</v>
+        <v>1165</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -23635,13 +23673,13 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C56">
         <v>1</v>
       </c>
-      <c r="D56" t="s">
-        <v>1324</v>
+      <c r="D56" s="6" t="s">
+        <v>1315</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -23649,13 +23687,13 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C57">
         <v>1</v>
       </c>
       <c r="D57" t="s">
-        <v>1325</v>
+        <v>1316</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -23663,13 +23701,13 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C58">
         <v>1</v>
       </c>
       <c r="D58" t="s">
-        <v>1326</v>
+        <v>1317</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -23677,13 +23715,13 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C59">
         <v>1</v>
       </c>
       <c r="D59" t="s">
-        <v>1327</v>
+        <v>1318</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -23691,13 +23729,13 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C60">
         <v>1</v>
       </c>
       <c r="D60" t="s">
-        <v>1328</v>
+        <v>1319</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -23705,13 +23743,13 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C61">
         <v>1</v>
       </c>
       <c r="D61" t="s">
-        <v>1152</v>
+        <v>1320</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -23725,7 +23763,7 @@
         <v>1</v>
       </c>
       <c r="D62" t="s">
-        <v>1329</v>
+        <v>1263</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -23739,7 +23777,7 @@
         <v>1</v>
       </c>
       <c r="D63" t="s">
-        <v>1330</v>
+        <v>1321</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -23753,7 +23791,7 @@
         <v>1</v>
       </c>
       <c r="D64" t="s">
-        <v>1331</v>
+        <v>1322</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -23767,7 +23805,7 @@
         <v>1</v>
       </c>
       <c r="D65" t="s">
-        <v>1332</v>
+        <v>1323</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -23781,7 +23819,7 @@
         <v>1</v>
       </c>
       <c r="D66" t="s">
-        <v>1333</v>
+        <v>1324</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -23789,13 +23827,13 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C67">
         <v>1</v>
       </c>
-      <c r="D67" s="3" t="s">
-        <v>1264</v>
+      <c r="D67" t="s">
+        <v>1325</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -23803,13 +23841,13 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C68">
         <v>1</v>
       </c>
-      <c r="D68" s="3" t="s">
-        <v>1265</v>
+      <c r="D68" t="s">
+        <v>1326</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -23817,13 +23855,13 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C69">
         <v>1</v>
       </c>
-      <c r="D69" s="3" t="s">
-        <v>1266</v>
+      <c r="D69" t="s">
+        <v>1327</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -23831,13 +23869,13 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C70">
         <v>1</v>
       </c>
-      <c r="D70" s="3" t="s">
-        <v>1267</v>
+      <c r="D70" t="s">
+        <v>1328</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -23845,13 +23883,13 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C71">
         <v>1</v>
       </c>
       <c r="D71" t="s">
-        <v>1268</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -23859,13 +23897,13 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C72">
         <v>1</v>
       </c>
-      <c r="D72" s="3" t="s">
-        <v>1269</v>
+      <c r="D72" t="s">
+        <v>1329</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -23873,13 +23911,13 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C73">
         <v>1</v>
       </c>
       <c r="D73" t="s">
-        <v>1283</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -23887,13 +23925,13 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C74">
         <v>1</v>
       </c>
       <c r="D74" t="s">
-        <v>1284</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -23901,13 +23939,13 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C75">
         <v>1</v>
       </c>
       <c r="D75" t="s">
-        <v>1285</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -23915,13 +23953,13 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C76">
         <v>1</v>
       </c>
-      <c r="D76" s="3" t="s">
-        <v>1286</v>
+      <c r="D76" t="s">
+        <v>1333</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -23935,7 +23973,7 @@
         <v>1</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>1287</v>
+        <v>1264</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -23949,7 +23987,7 @@
         <v>1</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>742</v>
+        <v>1265</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -23963,7 +24001,7 @@
         <v>1</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>1288</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -23976,8 +24014,8 @@
       <c r="C80">
         <v>1</v>
       </c>
-      <c r="D80" t="s">
-        <v>1289</v>
+      <c r="D80" s="3" t="s">
+        <v>1267</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -23991,7 +24029,7 @@
         <v>1</v>
       </c>
       <c r="D81" t="s">
-        <v>1290</v>
+        <v>1268</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -23999,13 +24037,13 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C82">
-        <v>2</v>
-      </c>
-      <c r="D82" t="s">
-        <v>1277</v>
+        <v>1</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>1269</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -24013,13 +24051,13 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C83">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D83" t="s">
-        <v>1278</v>
+        <v>1283</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -24027,13 +24065,13 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C84">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D84" t="s">
-        <v>1279</v>
+        <v>1284</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -24041,13 +24079,13 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C85">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D85" t="s">
-        <v>1280</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -24055,13 +24093,13 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C86">
-        <v>2</v>
-      </c>
-      <c r="D86" t="s">
-        <v>1281</v>
+        <v>1</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>1286</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -24069,13 +24107,13 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C87">
-        <v>2</v>
-      </c>
-      <c r="D87" t="s">
-        <v>1282</v>
+        <v>1</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>1287</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -24083,13 +24121,13 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C88">
-        <v>2</v>
-      </c>
-      <c r="D88" t="s">
-        <v>1274</v>
+        <v>1</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>742</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -24097,13 +24135,13 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C89">
-        <v>2</v>
-      </c>
-      <c r="D89" t="s">
-        <v>1275</v>
+        <v>1</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>1288</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -24111,13 +24149,13 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C90">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D90" t="s">
-        <v>1276</v>
+        <v>1289</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -24125,13 +24163,13 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C91">
-        <v>2</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>1273</v>
+        <v>1</v>
+      </c>
+      <c r="D91" t="s">
+        <v>1290</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -24144,8 +24182,8 @@
       <c r="C92">
         <v>2</v>
       </c>
-      <c r="D92" s="3" t="s">
-        <v>1272</v>
+      <c r="D92" t="s">
+        <v>1277</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -24158,8 +24196,8 @@
       <c r="C93">
         <v>2</v>
       </c>
-      <c r="D93" s="3" t="s">
-        <v>1270</v>
+      <c r="D93" t="s">
+        <v>1278</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -24172,8 +24210,8 @@
       <c r="C94">
         <v>2</v>
       </c>
-      <c r="D94" s="3" t="s">
-        <v>1271</v>
+      <c r="D94" t="s">
+        <v>1279</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -24187,7 +24225,7 @@
         <v>2</v>
       </c>
       <c r="D95" t="s">
-        <v>245</v>
+        <v>1280</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -24201,7 +24239,7 @@
         <v>2</v>
       </c>
       <c r="D96" t="s">
-        <v>246</v>
+        <v>1281</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -24209,13 +24247,13 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>331</v>
+        <v>22</v>
       </c>
       <c r="C97">
         <v>2</v>
       </c>
       <c r="D97" t="s">
-        <v>1291</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -24223,13 +24261,13 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>331</v>
+        <v>22</v>
       </c>
       <c r="C98">
         <v>2</v>
       </c>
       <c r="D98" t="s">
-        <v>1292</v>
+        <v>1274</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -24237,13 +24275,13 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>331</v>
+        <v>22</v>
       </c>
       <c r="C99">
         <v>2</v>
       </c>
       <c r="D99" t="s">
-        <v>1293</v>
+        <v>1275</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -24251,13 +24289,13 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>331</v>
+        <v>22</v>
       </c>
       <c r="C100">
         <v>2</v>
       </c>
       <c r="D100" t="s">
-        <v>1294</v>
+        <v>1276</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -24265,13 +24303,13 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>331</v>
+        <v>22</v>
       </c>
       <c r="C101">
         <v>2</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>1295</v>
+        <v>1273</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -24279,13 +24317,13 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>331</v>
+        <v>22</v>
       </c>
       <c r="C102">
         <v>2</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>1296</v>
+        <v>1272</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -24293,13 +24331,13 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>331</v>
+        <v>22</v>
       </c>
       <c r="C103">
         <v>2</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>1297</v>
+        <v>1270</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -24307,13 +24345,13 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>331</v>
+        <v>22</v>
       </c>
       <c r="C104">
         <v>2</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>1298</v>
+        <v>1271</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -24321,13 +24359,13 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>331</v>
+        <v>22</v>
       </c>
       <c r="C105">
         <v>2</v>
       </c>
       <c r="D105" t="s">
-        <v>1299</v>
+        <v>245</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -24335,13 +24373,13 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>331</v>
+        <v>22</v>
       </c>
       <c r="C106">
         <v>2</v>
       </c>
       <c r="D106" t="s">
-        <v>1300</v>
+        <v>246</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -24355,7 +24393,7 @@
         <v>2</v>
       </c>
       <c r="D107" t="s">
-        <v>1301</v>
+        <v>1291</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -24369,7 +24407,7 @@
         <v>2</v>
       </c>
       <c r="D108" t="s">
-        <v>1302</v>
+        <v>1292</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -24383,7 +24421,7 @@
         <v>2</v>
       </c>
       <c r="D109" t="s">
-        <v>1303</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -24397,7 +24435,7 @@
         <v>2</v>
       </c>
       <c r="D110" t="s">
-        <v>1305</v>
+        <v>1294</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -24410,8 +24448,8 @@
       <c r="C111">
         <v>2</v>
       </c>
-      <c r="D111" t="s">
-        <v>1304</v>
+      <c r="D111" s="3" t="s">
+        <v>1295</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
@@ -24419,13 +24457,13 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>24</v>
+        <v>331</v>
       </c>
       <c r="C112">
         <v>2</v>
       </c>
-      <c r="D112" t="s">
-        <v>1334</v>
+      <c r="D112" s="3" t="s">
+        <v>1296</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
@@ -24433,13 +24471,13 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>24</v>
+        <v>331</v>
       </c>
       <c r="C113">
         <v>2</v>
       </c>
-      <c r="D113" t="s">
-        <v>1335</v>
+      <c r="D113" s="3" t="s">
+        <v>1297</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
@@ -24447,13 +24485,13 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>24</v>
+        <v>331</v>
       </c>
       <c r="C114">
         <v>2</v>
       </c>
-      <c r="D114" t="s">
-        <v>1328</v>
+      <c r="D114" s="3" t="s">
+        <v>1298</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
@@ -24461,13 +24499,13 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>24</v>
+        <v>331</v>
       </c>
       <c r="C115">
         <v>2</v>
       </c>
       <c r="D115" t="s">
-        <v>1336</v>
+        <v>1299</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
@@ -24475,13 +24513,13 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>24</v>
+        <v>331</v>
       </c>
       <c r="C116">
         <v>2</v>
       </c>
       <c r="D116" t="s">
-        <v>1337</v>
+        <v>1300</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
@@ -24489,13 +24527,13 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>24</v>
+        <v>331</v>
       </c>
       <c r="C117">
         <v>2</v>
       </c>
       <c r="D117" t="s">
-        <v>1338</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
@@ -24503,13 +24541,13 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>24</v>
+        <v>331</v>
       </c>
       <c r="C118">
         <v>2</v>
       </c>
       <c r="D118" t="s">
-        <v>1329</v>
+        <v>1302</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
@@ -24517,13 +24555,13 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>24</v>
+        <v>331</v>
       </c>
       <c r="C119">
         <v>2</v>
       </c>
       <c r="D119" t="s">
-        <v>1152</v>
+        <v>1303</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -24531,13 +24569,13 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>24</v>
+        <v>331</v>
       </c>
       <c r="C120">
         <v>2</v>
       </c>
       <c r="D120" t="s">
-        <v>1330</v>
+        <v>1305</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
@@ -24545,13 +24583,13 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>24</v>
+        <v>331</v>
       </c>
       <c r="C121">
         <v>2</v>
       </c>
       <c r="D121" t="s">
-        <v>1339</v>
+        <v>1304</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -24565,7 +24603,7 @@
         <v>2</v>
       </c>
       <c r="D122" t="s">
-        <v>1340</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
@@ -24579,7 +24617,7 @@
         <v>2</v>
       </c>
       <c r="D123" t="s">
-        <v>1341</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
@@ -24593,7 +24631,7 @@
         <v>2</v>
       </c>
       <c r="D124" t="s">
-        <v>1342</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
@@ -24607,7 +24645,7 @@
         <v>2</v>
       </c>
       <c r="D125" t="s">
-        <v>1343</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
@@ -24621,7 +24659,7 @@
         <v>2</v>
       </c>
       <c r="D126" t="s">
-        <v>1344</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -24629,13 +24667,13 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C127">
         <v>2</v>
       </c>
       <c r="D127" t="s">
-        <v>1350</v>
+        <v>1338</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
@@ -24643,13 +24681,13 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C128">
         <v>2</v>
       </c>
       <c r="D128" t="s">
-        <v>1351</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
@@ -24657,13 +24695,13 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C129">
         <v>2</v>
       </c>
       <c r="D129" t="s">
-        <v>1352</v>
+        <v>1152</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
@@ -24671,13 +24709,13 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C130">
         <v>2</v>
       </c>
       <c r="D130" t="s">
-        <v>1353</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -24685,13 +24723,13 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C131">
         <v>2</v>
       </c>
       <c r="D131" t="s">
-        <v>1354</v>
+        <v>1339</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
@@ -24699,13 +24737,13 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C132">
         <v>2</v>
       </c>
       <c r="D132" t="s">
-        <v>1355</v>
+        <v>1340</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
@@ -24713,13 +24751,13 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C133">
         <v>2</v>
       </c>
       <c r="D133" t="s">
-        <v>1356</v>
+        <v>1341</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
@@ -24727,13 +24765,13 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C134">
         <v>2</v>
       </c>
       <c r="D134" t="s">
-        <v>1357</v>
+        <v>1342</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -24741,13 +24779,13 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C135">
         <v>2</v>
       </c>
       <c r="D135" t="s">
-        <v>1358</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
@@ -24755,13 +24793,13 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C136">
         <v>2</v>
       </c>
       <c r="D136" t="s">
-        <v>1359</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
@@ -24775,7 +24813,7 @@
         <v>2</v>
       </c>
       <c r="D137" t="s">
-        <v>1360</v>
+        <v>1350</v>
       </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
@@ -24789,7 +24827,7 @@
         <v>2</v>
       </c>
       <c r="D138" t="s">
-        <v>1361</v>
+        <v>1351</v>
       </c>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
@@ -24803,7 +24841,7 @@
         <v>2</v>
       </c>
       <c r="D139" t="s">
-        <v>1362</v>
+        <v>1352</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
@@ -24817,7 +24855,7 @@
         <v>2</v>
       </c>
       <c r="D140" t="s">
-        <v>1363</v>
+        <v>1353</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
@@ -24831,7 +24869,7 @@
         <v>2</v>
       </c>
       <c r="D141" t="s">
-        <v>1364</v>
+        <v>1354</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
@@ -24839,13 +24877,13 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C142">
         <v>2</v>
       </c>
       <c r="D142" t="s">
-        <v>1345</v>
+        <v>1355</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
@@ -24853,13 +24891,13 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C143">
         <v>2</v>
       </c>
       <c r="D143" t="s">
-        <v>1346</v>
+        <v>1356</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
@@ -24867,13 +24905,13 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C144">
         <v>2</v>
       </c>
       <c r="D144" t="s">
-        <v>1347</v>
+        <v>1357</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
@@ -24881,13 +24919,13 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C145">
         <v>2</v>
       </c>
       <c r="D145" t="s">
-        <v>1348</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
@@ -24895,13 +24933,13 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C146">
         <v>2</v>
       </c>
       <c r="D146" t="s">
-        <v>1349</v>
+        <v>1359</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
@@ -24909,10 +24947,13 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C147">
         <v>2</v>
+      </c>
+      <c r="D147" t="s">
+        <v>1360</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
@@ -24920,10 +24961,13 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C148">
         <v>2</v>
+      </c>
+      <c r="D148" t="s">
+        <v>1361</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
@@ -24931,10 +24975,13 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C149">
         <v>2</v>
+      </c>
+      <c r="D149" t="s">
+        <v>1362</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
@@ -24942,10 +24989,13 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C150">
         <v>2</v>
+      </c>
+      <c r="D150" t="s">
+        <v>1363</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
@@ -24953,10 +25003,13 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C151">
         <v>2</v>
+      </c>
+      <c r="D151" t="s">
+        <v>1364</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
@@ -24969,6 +25022,9 @@
       <c r="C152">
         <v>2</v>
       </c>
+      <c r="D152" t="s">
+        <v>1345</v>
+      </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A153">
@@ -24980,6 +25036,9 @@
       <c r="C153">
         <v>2</v>
       </c>
+      <c r="D153" t="s">
+        <v>1346</v>
+      </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A154">
@@ -24991,6 +25050,9 @@
       <c r="C154">
         <v>2</v>
       </c>
+      <c r="D154" t="s">
+        <v>1347</v>
+      </c>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A155">
@@ -25002,6 +25064,9 @@
       <c r="C155">
         <v>2</v>
       </c>
+      <c r="D155" t="s">
+        <v>1348</v>
+      </c>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A156">
@@ -25013,19 +25078,19 @@
       <c r="C156">
         <v>2</v>
       </c>
+      <c r="D156" t="s">
+        <v>1349</v>
+      </c>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>1147</v>
+        <v>26</v>
       </c>
       <c r="C157">
         <v>2</v>
-      </c>
-      <c r="D157" t="s">
-        <v>1146</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -25033,7 +25098,7 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>1147</v>
+        <v>26</v>
       </c>
       <c r="C158">
         <v>2</v>
@@ -25044,7 +25109,7 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>1147</v>
+        <v>26</v>
       </c>
       <c r="C159">
         <v>2</v>
@@ -25055,79 +25120,79 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>1147</v>
+        <v>26</v>
       </c>
       <c r="C160">
         <v>2</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>1147</v>
+        <v>26</v>
       </c>
       <c r="C161">
         <v>2</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>1147</v>
+        <v>26</v>
       </c>
       <c r="C162">
         <v>2</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>1147</v>
+        <v>26</v>
       </c>
       <c r="C163">
         <v>2</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>1147</v>
+        <v>26</v>
       </c>
       <c r="C164">
         <v>2</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>1147</v>
+        <v>26</v>
       </c>
       <c r="C165">
         <v>2</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>1147</v>
+        <v>26</v>
       </c>
       <c r="C166">
         <v>2</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
@@ -25137,8 +25202,11 @@
       <c r="C167">
         <v>2</v>
       </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D167" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>167</v>
       </c>
@@ -25149,7 +25217,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>168</v>
       </c>
@@ -25160,7 +25228,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>169</v>
       </c>
@@ -25171,7 +25239,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>170</v>
       </c>
@@ -25182,59 +25250,59 @@
         <v>2</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>27</v>
+        <v>1147</v>
       </c>
       <c r="C172">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>27</v>
+        <v>1147</v>
       </c>
       <c r="C173">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>27</v>
+        <v>1147</v>
       </c>
       <c r="C174">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>27</v>
+        <v>1147</v>
       </c>
       <c r="C175">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>27</v>
+        <v>1147</v>
       </c>
       <c r="C176">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
@@ -25242,10 +25310,10 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>27</v>
+        <v>1147</v>
       </c>
       <c r="C177">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
@@ -25253,10 +25321,10 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>27</v>
+        <v>1147</v>
       </c>
       <c r="C178">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
@@ -25264,10 +25332,10 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>27</v>
+        <v>1147</v>
       </c>
       <c r="C179">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
@@ -25275,10 +25343,10 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>27</v>
+        <v>1147</v>
       </c>
       <c r="C180">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
@@ -25286,10 +25354,10 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>27</v>
+        <v>1147</v>
       </c>
       <c r="C181">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
@@ -25352,7 +25420,7 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C187">
         <v>3</v>
@@ -25363,7 +25431,7 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C188">
         <v>3</v>
@@ -25374,7 +25442,7 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C189">
         <v>3</v>
@@ -25385,7 +25453,7 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C190">
         <v>3</v>
@@ -25396,7 +25464,7 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C191">
         <v>3</v>
@@ -25407,7 +25475,7 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C192">
         <v>3</v>
@@ -25418,7 +25486,7 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C193">
         <v>3</v>
@@ -25429,7 +25497,7 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C194">
         <v>3</v>
@@ -25440,7 +25508,7 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C195">
         <v>3</v>
@@ -25451,7 +25519,7 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C196">
         <v>3</v>
@@ -25509,6 +25577,116 @@
         <v>28</v>
       </c>
       <c r="C201">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202">
+        <v>201</v>
+      </c>
+      <c r="B202" t="s">
+        <v>28</v>
+      </c>
+      <c r="C202">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203">
+        <v>202</v>
+      </c>
+      <c r="B203" t="s">
+        <v>28</v>
+      </c>
+      <c r="C203">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204">
+        <v>203</v>
+      </c>
+      <c r="B204" t="s">
+        <v>28</v>
+      </c>
+      <c r="C204">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205">
+        <v>204</v>
+      </c>
+      <c r="B205" t="s">
+        <v>28</v>
+      </c>
+      <c r="C205">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206">
+        <v>205</v>
+      </c>
+      <c r="B206" t="s">
+        <v>28</v>
+      </c>
+      <c r="C206">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207">
+        <v>206</v>
+      </c>
+      <c r="B207" t="s">
+        <v>28</v>
+      </c>
+      <c r="C207">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208">
+        <v>207</v>
+      </c>
+      <c r="B208" t="s">
+        <v>28</v>
+      </c>
+      <c r="C208">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209">
+        <v>208</v>
+      </c>
+      <c r="B209" t="s">
+        <v>28</v>
+      </c>
+      <c r="C209">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210">
+        <v>209</v>
+      </c>
+      <c r="B210" t="s">
+        <v>28</v>
+      </c>
+      <c r="C210">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211">
+        <v>210</v>
+      </c>
+      <c r="B211" t="s">
+        <v>28</v>
+      </c>
+      <c r="C211">
         <v>3</v>
       </c>
     </row>
@@ -25519,12 +25697,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C2E62695FE58D640AF8E92EA86808B07" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2c5c749c9797d09654032a6edcbf8287">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="915c154c-1470-46a8-b038-1496da6ff25f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="af1527dc3e50601e83d1345c236a4602" ns3:_="">
     <xsd:import namespace="915c154c-1470-46a8-b038-1496da6ff25f"/>
@@ -25670,7 +25842,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -25679,23 +25851,13 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DC388A3-3E8E-468D-B938-40CD1FB812C5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="915c154c-1470-46a8-b038-1496da6ff25f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85056FB0-2F52-4A75-80BF-C38F7C8CF209}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -25713,10 +25875,26 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4344FF14-EBFA-4C51-8BB6-D67423FD69A5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DC388A3-3E8E-468D-B938-40CD1FB812C5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="915c154c-1470-46a8-b038-1496da6ff25f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
WIP 65 questions na
</commit_message>
<xml_diff>
--- a/assets/excel/Minigames.xlsx
+++ b/assets/excel/Minigames.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEM\Documents\GitHub\CodexLearning\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAF1ED8-D80C-443C-B7A8-1FE542F895A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0570562-4F5D-4358-A30A-DFAE82C623F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="3" xr2:uid="{2F4D6A40-7D2F-4386-B1F7-728101A5D7AD}"/>
+    <workbookView xWindow="1110" yWindow="405" windowWidth="15825" windowHeight="9855" firstSheet="1" activeTab="3" xr2:uid="{2F4D6A40-7D2F-4386-B1F7-728101A5D7AD}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeRiddle" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7674" uniqueCount="1458">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8003" uniqueCount="1474">
   <si>
     <t>Stage 1</t>
   </si>
@@ -4953,9 +4953,6 @@
     <t>("JediLand"</t>
   </si>
   <si>
-    <t>Conditional Statement</t>
-  </si>
-  <si>
     <t>((1 + 1)</t>
   </si>
   <si>
@@ -5119,6 +5116,57 @@
   </si>
   <si>
     <t>"C"</t>
+  </si>
+  <si>
+    <t>i=0</t>
+  </si>
+  <si>
+    <t>i&lt;5</t>
+  </si>
+  <si>
+    <t>i++)</t>
+  </si>
+  <si>
+    <t>while</t>
+  </si>
+  <si>
+    <t>(i&lt;5)</t>
+  </si>
+  <si>
+    <t>do</t>
+  </si>
+  <si>
+    <t>(i)</t>
+  </si>
+  <si>
+    <t>(i==2)</t>
+  </si>
+  <si>
+    <t>array</t>
+  </si>
+  <si>
+    <t>"is"</t>
+  </si>
+  <si>
+    <t>"in"</t>
+  </si>
+  <si>
+    <t>"Jediland"</t>
+  </si>
+  <si>
+    <t>i&lt;</t>
+  </si>
+  <si>
+    <t>(array[i])</t>
+  </si>
+  <si>
+    <t>"going"</t>
+  </si>
+  <si>
+    <t>"to"</t>
+  </si>
+  <si>
+    <t>"Jedischool"</t>
   </si>
 </sst>
 </file>
@@ -26578,10 +26626,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63F261A1-0426-462C-979C-1324696FD2FB}">
-  <dimension ref="A1:O442"/>
+  <dimension ref="A1:O522"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A409" workbookViewId="0">
-      <selection activeCell="J419" sqref="J419"/>
+    <sheetView tabSelected="1" topLeftCell="A275" workbookViewId="0">
+      <selection activeCell="B289" sqref="B289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -27107,7 +27155,7 @@
         <v>1196</v>
       </c>
       <c r="J26" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="K26" t="s">
         <v>264</v>
@@ -28354,7 +28402,7 @@
         <v>795</v>
       </c>
       <c r="F87" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="G87" t="s">
         <v>264</v>
@@ -28442,7 +28490,7 @@
         <v>795</v>
       </c>
       <c r="F92" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="G92" t="s">
         <v>264</v>
@@ -28530,7 +28578,7 @@
         <v>795</v>
       </c>
       <c r="F97" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="G97" t="s">
         <v>264</v>
@@ -28644,7 +28692,7 @@
         <v>795</v>
       </c>
       <c r="F103" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="G103" t="s">
         <v>264</v>
@@ -28664,7 +28712,7 @@
         <v>795</v>
       </c>
       <c r="F104" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="G104" t="s">
         <v>264</v>
@@ -28676,7 +28724,7 @@
         <v>264</v>
       </c>
       <c r="J104" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="K104" t="s">
         <v>157</v>
@@ -28778,7 +28826,7 @@
         <v>795</v>
       </c>
       <c r="F110" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="G110" t="s">
         <v>264</v>
@@ -28798,7 +28846,7 @@
         <v>795</v>
       </c>
       <c r="F111" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="G111" t="s">
         <v>264</v>
@@ -28906,7 +28954,7 @@
         <v>795</v>
       </c>
       <c r="F117" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="G117" t="s">
         <v>264</v>
@@ -28932,7 +28980,7 @@
         <v>795</v>
       </c>
       <c r="F118" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="G118" t="s">
         <v>264</v>
@@ -28944,7 +28992,7 @@
         <v>264</v>
       </c>
       <c r="J118" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="K118" t="s">
         <v>157</v>
@@ -29066,7 +29114,7 @@
         <v>795</v>
       </c>
       <c r="F125" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="G125" t="s">
         <v>264</v>
@@ -29086,7 +29134,7 @@
         <v>795</v>
       </c>
       <c r="F126" t="s">
-        <v>1422</v>
+        <v>1421</v>
       </c>
       <c r="G126" t="s">
         <v>264</v>
@@ -29112,7 +29160,7 @@
         <v>795</v>
       </c>
       <c r="F127" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="G127" t="s">
         <v>264</v>
@@ -29124,7 +29172,7 @@
         <v>264</v>
       </c>
       <c r="J127" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="K127" t="s">
         <v>157</v>
@@ -29226,7 +29274,7 @@
         <v>795</v>
       </c>
       <c r="F133" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="G133" t="s">
         <v>264</v>
@@ -29246,7 +29294,7 @@
         <v>795</v>
       </c>
       <c r="F134" t="s">
-        <v>1421</v>
+        <v>1420</v>
       </c>
       <c r="G134" t="s">
         <v>264</v>
@@ -29368,7 +29416,7 @@
         <v>795</v>
       </c>
       <c r="F141" t="s">
-        <v>1420</v>
+        <v>1419</v>
       </c>
       <c r="G141" t="s">
         <v>264</v>
@@ -29391,7 +29439,7 @@
         <v>795</v>
       </c>
       <c r="F142" t="s">
-        <v>1419</v>
+        <v>1418</v>
       </c>
       <c r="G142" t="s">
         <v>264</v>
@@ -29403,7 +29451,7 @@
         <v>264</v>
       </c>
       <c r="J142" t="s">
-        <v>1418</v>
+        <v>1417</v>
       </c>
       <c r="K142" t="s">
         <v>157</v>
@@ -29571,7 +29619,7 @@
         <v>795</v>
       </c>
       <c r="F151" t="s">
-        <v>1417</v>
+        <v>1416</v>
       </c>
       <c r="G151" t="s">
         <v>264</v>
@@ -29705,7 +29753,7 @@
         <v>795</v>
       </c>
       <c r="F158" t="s">
-        <v>1415</v>
+        <v>1414</v>
       </c>
       <c r="G158" t="s">
         <v>264</v>
@@ -29731,7 +29779,7 @@
         <v>795</v>
       </c>
       <c r="F159" t="s">
-        <v>1416</v>
+        <v>1415</v>
       </c>
       <c r="G159" t="s">
         <v>264</v>
@@ -31093,7 +31141,7 @@
         <v>240</v>
       </c>
       <c r="H231" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="I231" t="s">
         <v>157</v>
@@ -31130,7 +31178,7 @@
         <v>191</v>
       </c>
       <c r="F233" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="G233" t="s">
         <v>240</v>
@@ -31156,7 +31204,7 @@
         <v>264</v>
       </c>
       <c r="H234" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="I234" t="s">
         <v>264</v>
@@ -31182,7 +31230,7 @@
         <v>264</v>
       </c>
       <c r="H235" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="I235" t="s">
         <v>264</v>
@@ -31208,7 +31256,7 @@
         <v>264</v>
       </c>
       <c r="H236" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="I236" t="s">
         <v>264</v>
@@ -31296,7 +31344,7 @@
         <v>190</v>
       </c>
       <c r="F241" t="s">
-        <v>1411</v>
+        <v>1410</v>
       </c>
       <c r="G241" t="s">
         <v>240</v>
@@ -31345,19 +31393,19 @@
         <v>795</v>
       </c>
       <c r="F243" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="G243" t="s">
         <v>264</v>
       </c>
       <c r="H243" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="I243" t="s">
         <v>264</v>
       </c>
       <c r="J243" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="K243" t="s">
         <v>157</v>
@@ -31371,19 +31419,19 @@
         <v>795</v>
       </c>
       <c r="F244" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="G244" t="s">
         <v>264</v>
       </c>
       <c r="H244" t="s">
-        <v>1414</v>
+        <v>1413</v>
       </c>
       <c r="I244" t="s">
         <v>264</v>
       </c>
       <c r="J244" t="s">
-        <v>1413</v>
+        <v>1412</v>
       </c>
       <c r="K244" t="s">
         <v>157</v>
@@ -31397,13 +31445,13 @@
         <v>795</v>
       </c>
       <c r="F245" t="s">
-        <v>1412</v>
+        <v>1411</v>
       </c>
       <c r="G245" t="s">
         <v>264</v>
       </c>
       <c r="H245" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="I245" t="s">
         <v>264</v>
@@ -31471,13 +31519,13 @@
         <v>795</v>
       </c>
       <c r="F249" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="G249" t="s">
         <v>264</v>
       </c>
       <c r="H249" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="I249" t="s">
         <v>157</v>
@@ -31491,13 +31539,13 @@
         <v>795</v>
       </c>
       <c r="F250" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="G250" t="s">
         <v>264</v>
       </c>
       <c r="H250" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="I250" t="s">
         <v>157</v>
@@ -31559,13 +31607,13 @@
         <v>795</v>
       </c>
       <c r="F254" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="G254" t="s">
         <v>264</v>
       </c>
       <c r="H254" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="I254" t="s">
         <v>157</v>
@@ -31579,13 +31627,13 @@
         <v>795</v>
       </c>
       <c r="F255" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="G255" t="s">
         <v>264</v>
       </c>
       <c r="H255" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="I255" t="s">
         <v>157</v>
@@ -31667,7 +31715,7 @@
         <v>795</v>
       </c>
       <c r="F260" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="G260" t="s">
         <v>157</v>
@@ -31695,7 +31743,7 @@
         <v>795</v>
       </c>
       <c r="F262" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="G262" t="s">
         <v>157</v>
@@ -31777,7 +31825,7 @@
         <v>795</v>
       </c>
       <c r="F267" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="G267" t="s">
         <v>157</v>
@@ -31805,7 +31853,7 @@
         <v>795</v>
       </c>
       <c r="F269" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="G269" t="s">
         <v>157</v>
@@ -31887,19 +31935,19 @@
         <v>795</v>
       </c>
       <c r="F274" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="G274" t="s">
         <v>264</v>
       </c>
       <c r="H274" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="I274" t="s">
         <v>806</v>
       </c>
       <c r="J274" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="K274" t="s">
         <v>157</v>
@@ -31927,7 +31975,7 @@
         <v>795</v>
       </c>
       <c r="F276" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="G276" t="s">
         <v>157</v>
@@ -32052,19 +32100,19 @@
         <v>795</v>
       </c>
       <c r="F283" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="G283" t="s">
         <v>259</v>
       </c>
       <c r="H283" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
       <c r="I283" t="s">
         <v>806</v>
       </c>
       <c r="J283" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="K283" t="s">
         <v>157</v>
@@ -32078,7 +32126,7 @@
         <v>795</v>
       </c>
       <c r="F284" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="G284" t="s">
         <v>157</v>
@@ -32092,7 +32140,7 @@
         <v>795</v>
       </c>
       <c r="F285" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
       <c r="G285" t="s">
         <v>157</v>
@@ -32154,7 +32202,7 @@
         <v>43</v>
       </c>
       <c r="B289" t="s">
-        <v>1402</v>
+        <v>22</v>
       </c>
       <c r="C289" t="s">
         <v>6</v>
@@ -32228,7 +32276,7 @@
         <v>795</v>
       </c>
       <c r="F293" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="G293" t="s">
         <v>157</v>
@@ -32256,7 +32304,7 @@
         <v>795</v>
       </c>
       <c r="F295" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="G295" t="s">
         <v>157</v>
@@ -32286,7 +32334,7 @@
         <v>44</v>
       </c>
       <c r="B298" t="s">
-        <v>1402</v>
+        <v>22</v>
       </c>
       <c r="C298" t="s">
         <v>6</v>
@@ -32360,7 +32408,7 @@
         <v>795</v>
       </c>
       <c r="F302" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
       <c r="G302" t="s">
         <v>157</v>
@@ -32388,7 +32436,7 @@
         <v>795</v>
       </c>
       <c r="F304" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="G304" t="s">
         <v>157</v>
@@ -32427,7 +32475,7 @@
         <v>45</v>
       </c>
       <c r="B307" t="s">
-        <v>1402</v>
+        <v>22</v>
       </c>
       <c r="C307" t="s">
         <v>7</v>
@@ -32507,7 +32555,7 @@
         <v>280</v>
       </c>
       <c r="F311" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="G311" t="s">
         <v>158</v>
@@ -32527,7 +32575,7 @@
         <v>795</v>
       </c>
       <c r="F312" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="G312" t="s">
         <v>157</v>
@@ -32555,7 +32603,7 @@
         <v>795</v>
       </c>
       <c r="F314" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="G314" t="s">
         <v>157</v>
@@ -32580,7 +32628,7 @@
         <v>46</v>
       </c>
       <c r="B316" t="s">
-        <v>1402</v>
+        <v>22</v>
       </c>
       <c r="C316" t="s">
         <v>7</v>
@@ -32660,7 +32708,7 @@
         <v>280</v>
       </c>
       <c r="F320" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
       <c r="G320" t="s">
         <v>820</v>
@@ -32680,7 +32728,7 @@
         <v>795</v>
       </c>
       <c r="F321" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="G321" t="s">
         <v>157</v>
@@ -32708,7 +32756,7 @@
         <v>795</v>
       </c>
       <c r="F323" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="G323" t="s">
         <v>157</v>
@@ -32733,7 +32781,7 @@
         <v>47</v>
       </c>
       <c r="B325" t="s">
-        <v>1402</v>
+        <v>22</v>
       </c>
       <c r="C325" t="s">
         <v>8</v>
@@ -32813,7 +32861,7 @@
         <v>191</v>
       </c>
       <c r="F329" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="G329" t="s">
         <v>240</v>
@@ -32833,13 +32881,13 @@
         <v>280</v>
       </c>
       <c r="F330" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="G330" t="s">
         <v>158</v>
       </c>
       <c r="H330" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="I330" t="s">
         <v>802</v>
@@ -32853,7 +32901,7 @@
         <v>795</v>
       </c>
       <c r="F331" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="G331" t="s">
         <v>157</v>
@@ -32867,10 +32915,10 @@
     </row>
     <row r="332" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E332" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="F332" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="G332" t="s">
         <v>158</v>
@@ -32890,7 +32938,7 @@
         <v>795</v>
       </c>
       <c r="F333" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="G333" t="s">
         <v>157</v>
@@ -32918,7 +32966,7 @@
         <v>795</v>
       </c>
       <c r="F335" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="G335" t="s">
         <v>157</v>
@@ -32943,7 +32991,7 @@
         <v>48</v>
       </c>
       <c r="B337" t="s">
-        <v>1402</v>
+        <v>22</v>
       </c>
       <c r="C337" t="s">
         <v>8</v>
@@ -33023,7 +33071,7 @@
         <v>191</v>
       </c>
       <c r="F341" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="G341" t="s">
         <v>240</v>
@@ -33043,13 +33091,13 @@
         <v>280</v>
       </c>
       <c r="F342" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="G342" t="s">
         <v>158</v>
       </c>
       <c r="H342" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="I342" t="s">
         <v>802</v>
@@ -33063,7 +33111,7 @@
         <v>795</v>
       </c>
       <c r="F343" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="G343" t="s">
         <v>157</v>
@@ -33077,10 +33125,10 @@
     </row>
     <row r="344" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E344" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="F344" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="G344" t="s">
         <v>820</v>
@@ -33100,7 +33148,7 @@
         <v>795</v>
       </c>
       <c r="F345" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
       <c r="G345" t="s">
         <v>157</v>
@@ -33128,7 +33176,7 @@
         <v>795</v>
       </c>
       <c r="F347" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="G347" t="s">
         <v>157</v>
@@ -33156,7 +33204,7 @@
         <v>49</v>
       </c>
       <c r="B349" t="s">
-        <v>1402</v>
+        <v>22</v>
       </c>
       <c r="C349" t="s">
         <v>6</v>
@@ -33196,7 +33244,7 @@
         <v>192</v>
       </c>
       <c r="F351" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="G351" t="s">
         <v>240</v>
@@ -33216,7 +33264,7 @@
         <v>285</v>
       </c>
       <c r="F352" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="G352" t="s">
         <v>802</v>
@@ -33227,7 +33275,7 @@
     </row>
     <row r="353" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E353" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="F353" s="2" t="s">
         <v>1366</v>
@@ -33244,7 +33292,7 @@
         <v>795</v>
       </c>
       <c r="F354" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="G354" t="s">
         <v>157</v>
@@ -33280,7 +33328,7 @@
         <v>795</v>
       </c>
       <c r="F357" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="G357" t="s">
         <v>157</v>
@@ -33316,7 +33364,7 @@
         <v>50</v>
       </c>
       <c r="B360" t="s">
-        <v>1402</v>
+        <v>22</v>
       </c>
       <c r="C360" t="s">
         <v>6</v>
@@ -33356,13 +33404,13 @@
         <v>192</v>
       </c>
       <c r="F362" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="G362" t="s">
         <v>240</v>
       </c>
       <c r="H362" s="2" t="s">
-        <v>1447</v>
+        <v>1446</v>
       </c>
       <c r="I362" t="s">
         <v>157</v>
@@ -33376,7 +33424,7 @@
         <v>285</v>
       </c>
       <c r="F363" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="G363" t="s">
         <v>802</v>
@@ -33387,7 +33435,7 @@
     </row>
     <row r="364" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E364" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="F364" s="2" t="s">
         <v>1366</v>
@@ -33404,7 +33452,7 @@
         <v>795</v>
       </c>
       <c r="F365" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="G365" t="s">
         <v>157</v>
@@ -33440,7 +33488,7 @@
         <v>795</v>
       </c>
       <c r="F368" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="G368" t="s">
         <v>157</v>
@@ -33476,7 +33524,7 @@
         <v>51</v>
       </c>
       <c r="B371" t="s">
-        <v>1402</v>
+        <v>22</v>
       </c>
       <c r="C371" t="s">
         <v>7</v>
@@ -33516,13 +33564,13 @@
         <v>143</v>
       </c>
       <c r="F373" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="G373" t="s">
         <v>240</v>
       </c>
       <c r="H373" s="2" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="I373" t="s">
         <v>157</v>
@@ -33536,7 +33584,7 @@
         <v>285</v>
       </c>
       <c r="F374" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="G374" t="s">
         <v>802</v>
@@ -33547,10 +33595,10 @@
     </row>
     <row r="375" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E375" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="F375" s="2" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="G375" t="s">
         <v>1067</v>
@@ -33564,7 +33612,7 @@
         <v>795</v>
       </c>
       <c r="F376" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="G376" t="s">
         <v>157</v>
@@ -33586,10 +33634,10 @@
     </row>
     <row r="378" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E378" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="F378" s="2" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="G378" t="s">
         <v>1067</v>
@@ -33603,7 +33651,7 @@
         <v>795</v>
       </c>
       <c r="F379" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="G379" t="s">
         <v>157</v>
@@ -33639,7 +33687,7 @@
         <v>795</v>
       </c>
       <c r="F382" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="G382" t="s">
         <v>157</v>
@@ -33675,7 +33723,7 @@
         <v>52</v>
       </c>
       <c r="B385" t="s">
-        <v>1402</v>
+        <v>22</v>
       </c>
       <c r="C385" t="s">
         <v>7</v>
@@ -33715,13 +33763,13 @@
         <v>143</v>
       </c>
       <c r="F387" t="s">
-        <v>1449</v>
+        <v>1448</v>
       </c>
       <c r="G387" t="s">
         <v>240</v>
       </c>
       <c r="H387" s="2" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="I387" t="s">
         <v>157</v>
@@ -33735,7 +33783,7 @@
         <v>285</v>
       </c>
       <c r="F388" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="G388" t="s">
         <v>802</v>
@@ -33746,10 +33794,10 @@
     </row>
     <row r="389" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E389" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="F389" s="2" t="s">
-        <v>1450</v>
+        <v>1449</v>
       </c>
       <c r="G389" t="s">
         <v>1067</v>
@@ -33763,7 +33811,7 @@
         <v>795</v>
       </c>
       <c r="F390" t="s">
-        <v>1453</v>
+        <v>1452</v>
       </c>
       <c r="G390" t="s">
         <v>157</v>
@@ -33785,10 +33833,10 @@
     </row>
     <row r="392" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E392" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="F392" s="2" t="s">
-        <v>1452</v>
+        <v>1451</v>
       </c>
       <c r="G392" t="s">
         <v>1067</v>
@@ -33802,7 +33850,7 @@
         <v>795</v>
       </c>
       <c r="F393" t="s">
-        <v>1454</v>
+        <v>1453</v>
       </c>
       <c r="G393" t="s">
         <v>157</v>
@@ -33838,7 +33886,7 @@
         <v>795</v>
       </c>
       <c r="F396" t="s">
-        <v>1451</v>
+        <v>1450</v>
       </c>
       <c r="G396" t="s">
         <v>157</v>
@@ -33874,7 +33922,7 @@
         <v>53</v>
       </c>
       <c r="B399" t="s">
-        <v>1402</v>
+        <v>22</v>
       </c>
       <c r="C399" t="s">
         <v>8</v>
@@ -33914,13 +33962,13 @@
         <v>143</v>
       </c>
       <c r="F401" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="G401" t="s">
         <v>240</v>
       </c>
       <c r="H401" s="2" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="I401" t="s">
         <v>157</v>
@@ -33934,7 +33982,7 @@
         <v>285</v>
       </c>
       <c r="F402" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="G402" t="s">
         <v>802</v>
@@ -33945,10 +33993,10 @@
     </row>
     <row r="403" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E403" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="F403" s="2" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="G403" t="s">
         <v>1067</v>
@@ -33962,7 +34010,7 @@
         <v>795</v>
       </c>
       <c r="F404" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="G404" t="s">
         <v>157</v>
@@ -33984,10 +34032,10 @@
     </row>
     <row r="406" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E406" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="F406" s="2" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="G406" t="s">
         <v>1067</v>
@@ -34001,7 +34049,7 @@
         <v>795</v>
       </c>
       <c r="F407" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="G407" t="s">
         <v>157</v>
@@ -34037,7 +34085,7 @@
         <v>795</v>
       </c>
       <c r="F410" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="G410" t="s">
         <v>157</v>
@@ -34073,7 +34121,7 @@
         <v>54</v>
       </c>
       <c r="B413" t="s">
-        <v>1402</v>
+        <v>22</v>
       </c>
       <c r="C413" t="s">
         <v>8</v>
@@ -34113,13 +34161,13 @@
         <v>143</v>
       </c>
       <c r="F415" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="G415" t="s">
         <v>240</v>
       </c>
       <c r="H415" s="2" t="s">
-        <v>1457</v>
+        <v>1456</v>
       </c>
       <c r="I415" t="s">
         <v>157</v>
@@ -34133,7 +34181,7 @@
         <v>285</v>
       </c>
       <c r="F416" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="G416" t="s">
         <v>802</v>
@@ -34144,10 +34192,10 @@
     </row>
     <row r="417" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E417" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="F417" s="2" t="s">
-        <v>1455</v>
+        <v>1454</v>
       </c>
       <c r="G417" t="s">
         <v>1067</v>
@@ -34161,7 +34209,7 @@
         <v>795</v>
       </c>
       <c r="F418" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="G418" t="s">
         <v>157</v>
@@ -34183,10 +34231,10 @@
     </row>
     <row r="420" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E420" t="s">
-        <v>1444</v>
+        <v>1443</v>
       </c>
       <c r="F420" s="2" t="s">
-        <v>1456</v>
+        <v>1455</v>
       </c>
       <c r="G420" t="s">
         <v>1067</v>
@@ -34200,7 +34248,7 @@
         <v>795</v>
       </c>
       <c r="F421" t="s">
-        <v>1446</v>
+        <v>1445</v>
       </c>
       <c r="G421" t="s">
         <v>157</v>
@@ -34236,7 +34284,7 @@
         <v>795</v>
       </c>
       <c r="F424" t="s">
-        <v>1448</v>
+        <v>1447</v>
       </c>
       <c r="G424" t="s">
         <v>157</v>
@@ -34309,28 +34357,28 @@
     </row>
     <row r="429" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E429" t="s">
-        <v>1194</v>
+        <v>286</v>
       </c>
       <c r="F429" t="s">
-        <v>1198</v>
+        <v>1248</v>
       </c>
       <c r="G429" t="s">
-        <v>1195</v>
+        <v>1457</v>
       </c>
       <c r="H429" t="s">
-        <v>1198</v>
+        <v>157</v>
       </c>
       <c r="I429" t="s">
-        <v>1196</v>
+        <v>1458</v>
       </c>
       <c r="J429" t="s">
-        <v>1197</v>
+        <v>157</v>
       </c>
       <c r="K429" t="s">
-        <v>157</v>
+        <v>1459</v>
       </c>
       <c r="L429" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="M429" t="s">
         <v>797</v>
@@ -34338,228 +34386,1435 @@
     </row>
     <row r="430" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E430" t="s">
-        <v>138</v>
+        <v>795</v>
+      </c>
+      <c r="F430" t="s">
+        <v>1395</v>
+      </c>
+      <c r="G430" t="s">
+        <v>157</v>
+      </c>
+      <c r="H430" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="431" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A431">
-        <v>56</v>
-      </c>
-      <c r="B431" t="s">
-        <v>23</v>
-      </c>
-      <c r="C431" t="s">
-        <v>8</v>
-      </c>
-      <c r="D431">
-        <v>6</v>
-      </c>
       <c r="E431" t="s">
-        <v>137</v>
+        <v>804</v>
+      </c>
+      <c r="F431" t="s">
+        <v>804</v>
+      </c>
+      <c r="G431" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="432" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E432" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="433" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A433">
+        <v>56</v>
+      </c>
+      <c r="B433" t="s">
+        <v>23</v>
+      </c>
+      <c r="C433" t="s">
+        <v>6</v>
+      </c>
+      <c r="D433">
+        <v>6</v>
+      </c>
+      <c r="E433" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="434" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E434" t="s">
         <v>139</v>
       </c>
-      <c r="F432" t="s">
+      <c r="F434" t="s">
         <v>141</v>
       </c>
-      <c r="G432" t="s">
+      <c r="G434" t="s">
         <v>142</v>
       </c>
-      <c r="H432" t="s">
+      <c r="H434" t="s">
         <v>800</v>
       </c>
-      <c r="I432" t="s">
+      <c r="I434" t="s">
         <v>801</v>
       </c>
-      <c r="J432" t="s">
+      <c r="J434" t="s">
         <v>802</v>
       </c>
-      <c r="K432" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="433" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E433" t="s">
-        <v>1194</v>
-      </c>
-      <c r="F433" t="s">
-        <v>1198</v>
-      </c>
-      <c r="G433" t="s">
-        <v>1195</v>
-      </c>
-      <c r="H433" t="s">
-        <v>1198</v>
-      </c>
-      <c r="I433" t="s">
-        <v>1196</v>
-      </c>
-      <c r="J433" t="s">
-        <v>1197</v>
-      </c>
-      <c r="K433" t="s">
-        <v>157</v>
-      </c>
-      <c r="L433" t="s">
+      <c r="K434" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="435" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E435" t="s">
+        <v>191</v>
+      </c>
+      <c r="F435" t="s">
+        <v>844</v>
+      </c>
+      <c r="G435" t="s">
+        <v>240</v>
+      </c>
+      <c r="H435">
+        <v>0</v>
+      </c>
+      <c r="I435" t="s">
+        <v>157</v>
+      </c>
+      <c r="J435" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="436" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E436" t="s">
+        <v>1460</v>
+      </c>
+      <c r="F436" t="s">
+        <v>1461</v>
+      </c>
+      <c r="G436" t="s">
+        <v>802</v>
+      </c>
+      <c r="H436" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="437" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E437" t="s">
+        <v>795</v>
+      </c>
+      <c r="F437" t="s">
+        <v>1395</v>
+      </c>
+      <c r="G437" t="s">
+        <v>157</v>
+      </c>
+      <c r="H437" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="438" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E438" t="s">
+        <v>877</v>
+      </c>
+      <c r="F438" t="s">
+        <v>157</v>
+      </c>
+      <c r="G438" t="s">
         <v>804</v>
       </c>
-      <c r="M433" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="434" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E434" t="s">
+      <c r="H438" t="s">
+        <v>804</v>
+      </c>
+      <c r="I438" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="439" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E439" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="435" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A435">
+    <row r="440" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A440">
         <v>57</v>
       </c>
-      <c r="B435" t="s">
+      <c r="B440" t="s">
         <v>23</v>
       </c>
-      <c r="C435" t="s">
+      <c r="C440" t="s">
+        <v>6</v>
+      </c>
+      <c r="D440">
+        <v>6</v>
+      </c>
+      <c r="E440" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="441" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E441" t="s">
+        <v>139</v>
+      </c>
+      <c r="F441" t="s">
+        <v>141</v>
+      </c>
+      <c r="G441" t="s">
+        <v>142</v>
+      </c>
+      <c r="H441" t="s">
+        <v>800</v>
+      </c>
+      <c r="I441" t="s">
+        <v>801</v>
+      </c>
+      <c r="J441" t="s">
+        <v>802</v>
+      </c>
+      <c r="K441" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="442" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E442" t="s">
+        <v>191</v>
+      </c>
+      <c r="F442" t="s">
+        <v>844</v>
+      </c>
+      <c r="G442" t="s">
+        <v>240</v>
+      </c>
+      <c r="H442">
+        <v>0</v>
+      </c>
+      <c r="I442" t="s">
+        <v>157</v>
+      </c>
+      <c r="J442" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="443" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E443" t="s">
+        <v>1462</v>
+      </c>
+      <c r="F443" t="s">
+        <v>802</v>
+      </c>
+      <c r="G443" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="444" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E444" t="s">
+        <v>795</v>
+      </c>
+      <c r="F444" t="s">
+        <v>1395</v>
+      </c>
+      <c r="G444" t="s">
+        <v>157</v>
+      </c>
+      <c r="H444" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="445" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E445" t="s">
+        <v>877</v>
+      </c>
+      <c r="F445" t="s">
+        <v>157</v>
+      </c>
+      <c r="G445" t="s">
+        <v>804</v>
+      </c>
+      <c r="H445" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="446" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E446" t="s">
+        <v>1460</v>
+      </c>
+      <c r="F446" t="s">
+        <v>1461</v>
+      </c>
+      <c r="G446" t="s">
+        <v>157</v>
+      </c>
+      <c r="H446" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="447" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E447" t="s">
+        <v>804</v>
+      </c>
+      <c r="F447" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="448" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E448" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="449" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A449">
+        <v>58</v>
+      </c>
+      <c r="B449" t="s">
+        <v>23</v>
+      </c>
+      <c r="C449" t="s">
+        <v>7</v>
+      </c>
+      <c r="D449">
+        <v>6</v>
+      </c>
+      <c r="E449" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="450" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E450" t="s">
+        <v>139</v>
+      </c>
+      <c r="F450" t="s">
+        <v>141</v>
+      </c>
+      <c r="G450" t="s">
+        <v>142</v>
+      </c>
+      <c r="H450" t="s">
+        <v>800</v>
+      </c>
+      <c r="I450" t="s">
+        <v>801</v>
+      </c>
+      <c r="J450" t="s">
+        <v>802</v>
+      </c>
+      <c r="K450" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="451" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E451" t="s">
+        <v>286</v>
+      </c>
+      <c r="F451" t="s">
+        <v>1248</v>
+      </c>
+      <c r="G451" t="s">
+        <v>1457</v>
+      </c>
+      <c r="H451" t="s">
+        <v>157</v>
+      </c>
+      <c r="I451" t="s">
+        <v>1458</v>
+      </c>
+      <c r="J451" t="s">
+        <v>157</v>
+      </c>
+      <c r="K451" t="s">
+        <v>1459</v>
+      </c>
+      <c r="L451" t="s">
+        <v>802</v>
+      </c>
+      <c r="M451" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="452" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E452" t="s">
+        <v>795</v>
+      </c>
+      <c r="F452" t="s">
+        <v>1463</v>
+      </c>
+      <c r="G452" t="s">
+        <v>157</v>
+      </c>
+      <c r="H452" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="453" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E453" t="s">
+        <v>795</v>
+      </c>
+      <c r="F453" t="s">
+        <v>1395</v>
+      </c>
+      <c r="G453" t="s">
+        <v>157</v>
+      </c>
+      <c r="H453" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="454" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E454" t="s">
+        <v>804</v>
+      </c>
+      <c r="F454" t="s">
+        <v>804</v>
+      </c>
+      <c r="G454" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="455" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E455" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="456" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A456">
+        <v>59</v>
+      </c>
+      <c r="B456" t="s">
+        <v>23</v>
+      </c>
+      <c r="C456" t="s">
+        <v>7</v>
+      </c>
+      <c r="D456">
+        <v>6</v>
+      </c>
+      <c r="E456" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="457" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E457" t="s">
+        <v>139</v>
+      </c>
+      <c r="F457" t="s">
+        <v>141</v>
+      </c>
+      <c r="G457" t="s">
+        <v>142</v>
+      </c>
+      <c r="H457" t="s">
+        <v>800</v>
+      </c>
+      <c r="I457" t="s">
+        <v>801</v>
+      </c>
+      <c r="J457" t="s">
+        <v>802</v>
+      </c>
+      <c r="K457" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="458" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E458" t="s">
+        <v>191</v>
+      </c>
+      <c r="F458" t="s">
+        <v>844</v>
+      </c>
+      <c r="G458" t="s">
+        <v>240</v>
+      </c>
+      <c r="H458">
+        <v>0</v>
+      </c>
+      <c r="I458" t="s">
+        <v>157</v>
+      </c>
+      <c r="J458" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="459" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E459" t="s">
+        <v>1460</v>
+      </c>
+      <c r="F459" t="s">
+        <v>1461</v>
+      </c>
+      <c r="G459" t="s">
+        <v>802</v>
+      </c>
+      <c r="H459" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="460" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E460" t="s">
+        <v>795</v>
+      </c>
+      <c r="F460" t="s">
+        <v>1463</v>
+      </c>
+      <c r="G460" t="s">
+        <v>157</v>
+      </c>
+      <c r="H460" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="461" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E461" t="s">
+        <v>795</v>
+      </c>
+      <c r="F461" t="s">
+        <v>1395</v>
+      </c>
+      <c r="G461" t="s">
+        <v>157</v>
+      </c>
+      <c r="H461" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="462" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E462" t="s">
+        <v>877</v>
+      </c>
+      <c r="F462" t="s">
+        <v>157</v>
+      </c>
+      <c r="G462" t="s">
+        <v>804</v>
+      </c>
+      <c r="H462" t="s">
+        <v>804</v>
+      </c>
+      <c r="I462" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="463" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E463" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="464" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A464">
+        <v>60</v>
+      </c>
+      <c r="B464" t="s">
+        <v>23</v>
+      </c>
+      <c r="C464" t="s">
+        <v>7</v>
+      </c>
+      <c r="D464">
+        <v>6</v>
+      </c>
+      <c r="E464" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="465" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E465" t="s">
+        <v>139</v>
+      </c>
+      <c r="F465" t="s">
+        <v>141</v>
+      </c>
+      <c r="G465" t="s">
+        <v>142</v>
+      </c>
+      <c r="H465" t="s">
+        <v>800</v>
+      </c>
+      <c r="I465" t="s">
+        <v>801</v>
+      </c>
+      <c r="J465" t="s">
+        <v>802</v>
+      </c>
+      <c r="K465" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="466" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E466" t="s">
+        <v>191</v>
+      </c>
+      <c r="F466" t="s">
+        <v>844</v>
+      </c>
+      <c r="G466" t="s">
+        <v>240</v>
+      </c>
+      <c r="H466">
+        <v>0</v>
+      </c>
+      <c r="I466" t="s">
+        <v>157</v>
+      </c>
+      <c r="J466" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="467" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E467" t="s">
+        <v>1462</v>
+      </c>
+      <c r="F467" t="s">
+        <v>802</v>
+      </c>
+      <c r="G467" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="468" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E468" t="s">
+        <v>795</v>
+      </c>
+      <c r="F468" t="s">
+        <v>1463</v>
+      </c>
+      <c r="G468" t="s">
+        <v>157</v>
+      </c>
+      <c r="H468" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="469" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E469" t="s">
+        <v>795</v>
+      </c>
+      <c r="F469" t="s">
+        <v>1395</v>
+      </c>
+      <c r="G469" t="s">
+        <v>157</v>
+      </c>
+      <c r="H469" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="470" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E470" t="s">
+        <v>877</v>
+      </c>
+      <c r="F470" t="s">
+        <v>157</v>
+      </c>
+      <c r="G470" t="s">
+        <v>804</v>
+      </c>
+      <c r="H470" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="471" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E471" t="s">
+        <v>1460</v>
+      </c>
+      <c r="F471" t="s">
+        <v>1461</v>
+      </c>
+      <c r="G471" t="s">
+        <v>157</v>
+      </c>
+      <c r="H471" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="472" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E472" t="s">
+        <v>804</v>
+      </c>
+      <c r="F472" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="473" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E473" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="474" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A474">
+        <v>61</v>
+      </c>
+      <c r="B474" t="s">
+        <v>23</v>
+      </c>
+      <c r="C474" t="s">
         <v>8</v>
       </c>
-      <c r="D435">
+      <c r="D474">
         <v>6</v>
       </c>
-      <c r="E435" t="s">
+      <c r="E474" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="436" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E436" t="s">
+    <row r="475" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E475" t="s">
         <v>139</v>
       </c>
-      <c r="F436" t="s">
+      <c r="F475" t="s">
         <v>141</v>
       </c>
-      <c r="G436" t="s">
+      <c r="G475" t="s">
         <v>142</v>
       </c>
-      <c r="H436" t="s">
+      <c r="H475" t="s">
         <v>800</v>
       </c>
-      <c r="I436" t="s">
+      <c r="I475" t="s">
         <v>801</v>
       </c>
-      <c r="J436" t="s">
+      <c r="J475" t="s">
         <v>802</v>
       </c>
-      <c r="K436" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="437" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E437" t="s">
-        <v>1194</v>
-      </c>
-      <c r="F437" t="s">
-        <v>1198</v>
-      </c>
-      <c r="G437" t="s">
-        <v>1195</v>
-      </c>
-      <c r="H437" t="s">
-        <v>1198</v>
-      </c>
-      <c r="I437" t="s">
-        <v>1196</v>
-      </c>
-      <c r="J437" t="s">
-        <v>1197</v>
-      </c>
-      <c r="K437" t="s">
-        <v>157</v>
-      </c>
-      <c r="L437" t="s">
+      <c r="K475" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="476" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E476" t="s">
+        <v>286</v>
+      </c>
+      <c r="F476" t="s">
+        <v>1248</v>
+      </c>
+      <c r="G476" t="s">
+        <v>1457</v>
+      </c>
+      <c r="H476" t="s">
+        <v>157</v>
+      </c>
+      <c r="I476" t="s">
+        <v>1458</v>
+      </c>
+      <c r="J476" t="s">
+        <v>157</v>
+      </c>
+      <c r="K476" t="s">
+        <v>1459</v>
+      </c>
+      <c r="L476" t="s">
+        <v>802</v>
+      </c>
+      <c r="M476" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="477" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E477" t="s">
+        <v>795</v>
+      </c>
+      <c r="F477" t="s">
+        <v>1463</v>
+      </c>
+      <c r="G477" t="s">
+        <v>157</v>
+      </c>
+      <c r="H477" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="478" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E478" t="s">
+        <v>795</v>
+      </c>
+      <c r="F478" t="s">
+        <v>1395</v>
+      </c>
+      <c r="G478" t="s">
+        <v>157</v>
+      </c>
+      <c r="H478" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="479" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E479" t="s">
+        <v>280</v>
+      </c>
+      <c r="F479" t="s">
+        <v>1464</v>
+      </c>
+      <c r="G479" t="s">
+        <v>802</v>
+      </c>
+      <c r="H479" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="480" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E480" t="s">
+        <v>271</v>
+      </c>
+      <c r="F480" t="s">
+        <v>157</v>
+      </c>
+      <c r="G480" t="s">
         <v>804</v>
       </c>
-      <c r="M437" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="438" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E438" t="s">
+      <c r="H480" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="481" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E481" t="s">
+        <v>804</v>
+      </c>
+      <c r="F481" t="s">
+        <v>804</v>
+      </c>
+      <c r="G481" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="482" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E482" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="439" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A439">
-        <v>58</v>
-      </c>
-      <c r="B439" t="s">
+    <row r="483" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A483">
+        <v>62</v>
+      </c>
+      <c r="B483" t="s">
+        <v>23</v>
+      </c>
+      <c r="C483" t="s">
+        <v>8</v>
+      </c>
+      <c r="D483">
+        <v>6</v>
+      </c>
+      <c r="E483" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="484" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E484" t="s">
+        <v>139</v>
+      </c>
+      <c r="F484" t="s">
+        <v>141</v>
+      </c>
+      <c r="G484" t="s">
+        <v>142</v>
+      </c>
+      <c r="H484" t="s">
+        <v>800</v>
+      </c>
+      <c r="I484" t="s">
+        <v>801</v>
+      </c>
+      <c r="J484" t="s">
+        <v>802</v>
+      </c>
+      <c r="K484" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="485" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E485" t="s">
+        <v>191</v>
+      </c>
+      <c r="F485" t="s">
+        <v>844</v>
+      </c>
+      <c r="G485" t="s">
+        <v>240</v>
+      </c>
+      <c r="H485">
+        <v>0</v>
+      </c>
+      <c r="I485" t="s">
+        <v>157</v>
+      </c>
+      <c r="J485" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="486" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E486" t="s">
+        <v>1460</v>
+      </c>
+      <c r="F486" t="s">
+        <v>1461</v>
+      </c>
+      <c r="G486" t="s">
+        <v>802</v>
+      </c>
+      <c r="H486" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="487" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E487" t="s">
+        <v>795</v>
+      </c>
+      <c r="F487" t="s">
+        <v>1463</v>
+      </c>
+      <c r="G487" t="s">
+        <v>157</v>
+      </c>
+      <c r="H487" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="488" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E488" t="s">
+        <v>795</v>
+      </c>
+      <c r="F488" t="s">
+        <v>1395</v>
+      </c>
+      <c r="G488" t="s">
+        <v>157</v>
+      </c>
+      <c r="H488" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="489" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E489" t="s">
+        <v>280</v>
+      </c>
+      <c r="F489" t="s">
+        <v>1464</v>
+      </c>
+      <c r="G489" t="s">
+        <v>802</v>
+      </c>
+      <c r="H489" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="490" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E490" t="s">
+        <v>271</v>
+      </c>
+      <c r="F490" t="s">
+        <v>157</v>
+      </c>
+      <c r="G490" t="s">
+        <v>804</v>
+      </c>
+      <c r="H490" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="491" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E491" t="s">
+        <v>877</v>
+      </c>
+      <c r="F491" t="s">
+        <v>157</v>
+      </c>
+      <c r="G491" t="s">
+        <v>804</v>
+      </c>
+      <c r="H491" t="s">
+        <v>804</v>
+      </c>
+      <c r="I491" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="492" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E492" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="493" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A493">
+        <v>63</v>
+      </c>
+      <c r="B493" t="s">
+        <v>23</v>
+      </c>
+      <c r="C493" t="s">
+        <v>8</v>
+      </c>
+      <c r="D493">
+        <v>6</v>
+      </c>
+      <c r="E493" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="494" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E494" t="s">
+        <v>139</v>
+      </c>
+      <c r="F494" t="s">
+        <v>141</v>
+      </c>
+      <c r="G494" t="s">
+        <v>142</v>
+      </c>
+      <c r="H494" t="s">
+        <v>800</v>
+      </c>
+      <c r="I494" t="s">
+        <v>801</v>
+      </c>
+      <c r="J494" t="s">
+        <v>802</v>
+      </c>
+      <c r="K494" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="495" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E495" t="s">
+        <v>191</v>
+      </c>
+      <c r="F495" t="s">
+        <v>844</v>
+      </c>
+      <c r="G495" t="s">
+        <v>240</v>
+      </c>
+      <c r="H495">
+        <v>0</v>
+      </c>
+      <c r="I495" t="s">
+        <v>157</v>
+      </c>
+      <c r="J495" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="496" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E496" t="s">
+        <v>1462</v>
+      </c>
+      <c r="F496" t="s">
+        <v>802</v>
+      </c>
+      <c r="G496" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="497" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E497" t="s">
+        <v>795</v>
+      </c>
+      <c r="F497" t="s">
+        <v>1463</v>
+      </c>
+      <c r="G497" t="s">
+        <v>157</v>
+      </c>
+      <c r="H497" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="498" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E498" t="s">
+        <v>795</v>
+      </c>
+      <c r="F498" t="s">
+        <v>1395</v>
+      </c>
+      <c r="G498" t="s">
+        <v>157</v>
+      </c>
+      <c r="H498" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="499" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E499" t="s">
+        <v>280</v>
+      </c>
+      <c r="F499" t="s">
+        <v>1464</v>
+      </c>
+      <c r="G499" t="s">
+        <v>802</v>
+      </c>
+      <c r="H499" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="500" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E500" t="s">
+        <v>271</v>
+      </c>
+      <c r="F500" t="s">
+        <v>157</v>
+      </c>
+      <c r="G500" t="s">
+        <v>804</v>
+      </c>
+      <c r="H500" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="501" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E501" t="s">
+        <v>877</v>
+      </c>
+      <c r="F501" t="s">
+        <v>157</v>
+      </c>
+      <c r="G501" t="s">
+        <v>804</v>
+      </c>
+      <c r="H501" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="502" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E502" t="s">
+        <v>1460</v>
+      </c>
+      <c r="F502" t="s">
+        <v>1461</v>
+      </c>
+      <c r="G502" t="s">
+        <v>157</v>
+      </c>
+      <c r="H502" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="503" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E503" t="s">
+        <v>804</v>
+      </c>
+      <c r="F503" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="504" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E504" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="505" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A505">
+        <v>64</v>
+      </c>
+      <c r="B505" t="s">
         <v>24</v>
       </c>
-      <c r="C439" t="s">
+      <c r="C505" t="s">
         <v>6</v>
       </c>
-      <c r="D439">
+      <c r="D505">
         <v>7</v>
       </c>
-      <c r="E439" t="s">
+      <c r="E505" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="440" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E440" t="s">
+    <row r="506" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E506" t="s">
         <v>139</v>
       </c>
-      <c r="F440" t="s">
+      <c r="F506" t="s">
         <v>141</v>
       </c>
-      <c r="G440" t="s">
+      <c r="G506" t="s">
         <v>142</v>
       </c>
-      <c r="H440" t="s">
+      <c r="H506" t="s">
         <v>800</v>
       </c>
-      <c r="I440" t="s">
+      <c r="I506" t="s">
         <v>801</v>
       </c>
-      <c r="J440" t="s">
+      <c r="J506" t="s">
         <v>802</v>
       </c>
-      <c r="K440" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="441" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E441" t="s">
-        <v>1194</v>
-      </c>
-      <c r="F441" t="s">
-        <v>1198</v>
-      </c>
-      <c r="G441" t="s">
-        <v>1195</v>
-      </c>
-      <c r="H441" t="s">
-        <v>1198</v>
-      </c>
-      <c r="I441" t="s">
-        <v>1196</v>
-      </c>
-      <c r="J441" t="s">
-        <v>1197</v>
-      </c>
-      <c r="K441" t="s">
-        <v>157</v>
-      </c>
-      <c r="L441" t="s">
+      <c r="K506" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="507" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E507" t="s">
+        <v>1068</v>
+      </c>
+      <c r="F507" t="s">
+        <v>1465</v>
+      </c>
+      <c r="G507" t="s">
+        <v>240</v>
+      </c>
+      <c r="H507" t="s">
+        <v>802</v>
+      </c>
+      <c r="I507" t="s">
+        <v>1346</v>
+      </c>
+      <c r="J507" t="s">
+        <v>263</v>
+      </c>
+      <c r="K507" t="s">
+        <v>1466</v>
+      </c>
+      <c r="L507" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="508" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E508" t="s">
+        <v>263</v>
+      </c>
+      <c r="F508" t="s">
+        <v>1467</v>
+      </c>
+      <c r="G508" t="s">
+        <v>263</v>
+      </c>
+      <c r="H508" t="s">
+        <v>1468</v>
+      </c>
+      <c r="I508" t="s">
         <v>804</v>
       </c>
-      <c r="M441" t="s">
-        <v>797</v>
-      </c>
-    </row>
-    <row r="442" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E442" t="s">
+      <c r="J508" t="s">
+        <v>157</v>
+      </c>
+      <c r="K508" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="509" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E509" t="s">
+        <v>286</v>
+      </c>
+      <c r="F509" t="s">
+        <v>1248</v>
+      </c>
+      <c r="G509" t="s">
+        <v>1457</v>
+      </c>
+      <c r="H509" t="s">
+        <v>157</v>
+      </c>
+      <c r="I509" t="s">
+        <v>1469</v>
+      </c>
+      <c r="J509" t="s">
+        <v>1465</v>
+      </c>
+      <c r="K509" t="s">
+        <v>817</v>
+      </c>
+      <c r="L509" t="s">
+        <v>365</v>
+      </c>
+      <c r="M509" t="s">
+        <v>157</v>
+      </c>
+      <c r="N509" t="s">
+        <v>1459</v>
+      </c>
+      <c r="O509" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="510" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E510" t="s">
+        <v>802</v>
+      </c>
+      <c r="F510" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="511" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E511" t="s">
+        <v>795</v>
+      </c>
+      <c r="F511" t="s">
+        <v>1470</v>
+      </c>
+      <c r="G511" t="s">
+        <v>157</v>
+      </c>
+      <c r="H511" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="512" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E512" t="s">
+        <v>804</v>
+      </c>
+      <c r="F512" t="s">
+        <v>804</v>
+      </c>
+      <c r="G512" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="513" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E513" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="514" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A514">
+        <v>65</v>
+      </c>
+      <c r="B514" t="s">
+        <v>24</v>
+      </c>
+      <c r="C514" t="s">
+        <v>6</v>
+      </c>
+      <c r="D514">
+        <v>7</v>
+      </c>
+      <c r="E514" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="515" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E515" t="s">
+        <v>139</v>
+      </c>
+      <c r="F515" t="s">
+        <v>141</v>
+      </c>
+      <c r="G515" t="s">
+        <v>142</v>
+      </c>
+      <c r="H515" t="s">
+        <v>800</v>
+      </c>
+      <c r="I515" t="s">
+        <v>801</v>
+      </c>
+      <c r="J515" t="s">
+        <v>802</v>
+      </c>
+      <c r="K515" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="516" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E516" t="s">
+        <v>1068</v>
+      </c>
+      <c r="F516" t="s">
+        <v>1465</v>
+      </c>
+      <c r="G516" t="s">
+        <v>240</v>
+      </c>
+      <c r="H516" t="s">
+        <v>802</v>
+      </c>
+      <c r="I516" t="s">
+        <v>1346</v>
+      </c>
+      <c r="J516" t="s">
+        <v>263</v>
+      </c>
+      <c r="K516" t="s">
+        <v>1466</v>
+      </c>
+      <c r="L516" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="517" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E517" t="s">
+        <v>263</v>
+      </c>
+      <c r="F517" t="s">
+        <v>1471</v>
+      </c>
+      <c r="G517" t="s">
+        <v>263</v>
+      </c>
+      <c r="H517" t="s">
+        <v>1472</v>
+      </c>
+      <c r="I517" t="s">
+        <v>263</v>
+      </c>
+      <c r="J517" t="s">
+        <v>1473</v>
+      </c>
+      <c r="K517" t="s">
+        <v>804</v>
+      </c>
+      <c r="L517" t="s">
+        <v>157</v>
+      </c>
+      <c r="M517" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="518" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E518" t="s">
+        <v>286</v>
+      </c>
+      <c r="F518" t="s">
+        <v>1248</v>
+      </c>
+      <c r="G518" t="s">
+        <v>1457</v>
+      </c>
+      <c r="H518" t="s">
+        <v>157</v>
+      </c>
+      <c r="I518" t="s">
+        <v>1469</v>
+      </c>
+      <c r="J518" t="s">
+        <v>1465</v>
+      </c>
+      <c r="K518" t="s">
+        <v>817</v>
+      </c>
+      <c r="L518" t="s">
+        <v>365</v>
+      </c>
+      <c r="M518" t="s">
+        <v>157</v>
+      </c>
+      <c r="N518" t="s">
+        <v>1459</v>
+      </c>
+      <c r="O518" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="519" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E519" t="s">
+        <v>802</v>
+      </c>
+      <c r="F519" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="520" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E520" t="s">
+        <v>795</v>
+      </c>
+      <c r="F520" t="s">
+        <v>1470</v>
+      </c>
+      <c r="G520" t="s">
+        <v>157</v>
+      </c>
+      <c r="H520" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="521" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E521" t="s">
+        <v>804</v>
+      </c>
+      <c r="F521" t="s">
+        <v>804</v>
+      </c>
+      <c r="G521" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="522" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E522" t="s">
         <v>138</v>
       </c>
     </row>

</xml_diff>

<commit_message>
its working <3 banishnumber wal apa
</commit_message>
<xml_diff>
--- a/assets/excel/Minigames.xlsx
+++ b/assets/excel/Minigames.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEM\Documents\GitHub\CodexLearning\assets\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1-SCHOOL\1-Prog\CodexLearning\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88AA8186-D206-447E-991D-D52E0477E0C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E7C5FD-DA7D-4F35-BC5E-E49DFCA0BE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{2F4D6A40-7D2F-4386-B1F7-728101A5D7AD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{2F4D6A40-7D2F-4386-B1F7-728101A5D7AD}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeRiddle" sheetId="4" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9260" uniqueCount="1534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9321" uniqueCount="1534">
   <si>
     <t>Stage 1</t>
   </si>
@@ -12628,8 +12628,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Y529"/>
   <sheetViews>
-    <sheetView topLeftCell="A511" workbookViewId="0">
-      <selection activeCell="E517" sqref="E517"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24010,8 +24010,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:D211"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A183" workbookViewId="0">
+      <selection activeCell="H169" sqref="H169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25498,7 +25498,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>330</v>
+        <v>23</v>
       </c>
       <c r="C107">
         <v>2</v>
@@ -25512,7 +25512,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>330</v>
+        <v>23</v>
       </c>
       <c r="C108">
         <v>2</v>
@@ -25526,7 +25526,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>330</v>
+        <v>23</v>
       </c>
       <c r="C109">
         <v>2</v>
@@ -25540,7 +25540,7 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>330</v>
+        <v>23</v>
       </c>
       <c r="C110">
         <v>2</v>
@@ -25554,7 +25554,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>330</v>
+        <v>23</v>
       </c>
       <c r="C111">
         <v>2</v>
@@ -25568,7 +25568,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>330</v>
+        <v>23</v>
       </c>
       <c r="C112">
         <v>2</v>
@@ -25582,7 +25582,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>330</v>
+        <v>23</v>
       </c>
       <c r="C113">
         <v>2</v>
@@ -25596,7 +25596,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>330</v>
+        <v>23</v>
       </c>
       <c r="C114">
         <v>2</v>
@@ -25610,7 +25610,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>330</v>
+        <v>23</v>
       </c>
       <c r="C115">
         <v>2</v>
@@ -25624,7 +25624,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>330</v>
+        <v>23</v>
       </c>
       <c r="C116">
         <v>2</v>
@@ -25638,7 +25638,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>330</v>
+        <v>23</v>
       </c>
       <c r="C117">
         <v>2</v>
@@ -25652,7 +25652,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>330</v>
+        <v>23</v>
       </c>
       <c r="C118">
         <v>2</v>
@@ -25666,7 +25666,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>330</v>
+        <v>23</v>
       </c>
       <c r="C119">
         <v>2</v>
@@ -25680,7 +25680,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>330</v>
+        <v>23</v>
       </c>
       <c r="C120">
         <v>2</v>
@@ -25694,7 +25694,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>330</v>
+        <v>23</v>
       </c>
       <c r="C121">
         <v>2</v>
@@ -26203,6 +26203,9 @@
       <c r="C157">
         <v>2</v>
       </c>
+      <c r="D157" t="s">
+        <v>1328</v>
+      </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A158">
@@ -26213,6 +26216,9 @@
       </c>
       <c r="C158">
         <v>2</v>
+      </c>
+      <c r="D158" t="s">
+        <v>1328</v>
       </c>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
@@ -26225,6 +26231,9 @@
       <c r="C159">
         <v>2</v>
       </c>
+      <c r="D159" t="s">
+        <v>1328</v>
+      </c>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A160">
@@ -26236,6 +26245,9 @@
       <c r="C160">
         <v>2</v>
       </c>
+      <c r="D160" t="s">
+        <v>1328</v>
+      </c>
     </row>
     <row r="161" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A161">
@@ -26247,6 +26259,9 @@
       <c r="C161">
         <v>2</v>
       </c>
+      <c r="D161" t="s">
+        <v>1328</v>
+      </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A162">
@@ -26258,6 +26273,9 @@
       <c r="C162">
         <v>2</v>
       </c>
+      <c r="D162" t="s">
+        <v>1328</v>
+      </c>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A163">
@@ -26269,6 +26287,9 @@
       <c r="C163">
         <v>2</v>
       </c>
+      <c r="D163" t="s">
+        <v>1328</v>
+      </c>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A164">
@@ -26280,6 +26301,9 @@
       <c r="C164">
         <v>2</v>
       </c>
+      <c r="D164" t="s">
+        <v>1328</v>
+      </c>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A165">
@@ -26291,6 +26315,9 @@
       <c r="C165">
         <v>2</v>
       </c>
+      <c r="D165" t="s">
+        <v>1328</v>
+      </c>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A166">
@@ -26302,19 +26329,22 @@
       <c r="C166">
         <v>2</v>
       </c>
+      <c r="D166" t="s">
+        <v>1328</v>
+      </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>1172</v>
+        <v>29</v>
       </c>
       <c r="C167">
         <v>2</v>
       </c>
       <c r="D167" t="s">
-        <v>1171</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
@@ -26322,10 +26352,13 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>1172</v>
+        <v>29</v>
       </c>
       <c r="C168">
         <v>2</v>
+      </c>
+      <c r="D168" t="s">
+        <v>1328</v>
       </c>
     </row>
     <row r="169" spans="1:4" x14ac:dyDescent="0.25">
@@ -26333,10 +26366,13 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>1172</v>
+        <v>29</v>
       </c>
       <c r="C169">
         <v>2</v>
+      </c>
+      <c r="D169" t="s">
+        <v>1328</v>
       </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
@@ -26344,10 +26380,13 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>1172</v>
+        <v>29</v>
       </c>
       <c r="C170">
         <v>2</v>
+      </c>
+      <c r="D170" t="s">
+        <v>1328</v>
       </c>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
@@ -26355,10 +26394,13 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>1172</v>
+        <v>29</v>
       </c>
       <c r="C171">
         <v>2</v>
+      </c>
+      <c r="D171" t="s">
+        <v>1328</v>
       </c>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
@@ -26366,10 +26408,13 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>1172</v>
+        <v>29</v>
       </c>
       <c r="C172">
         <v>2</v>
+      </c>
+      <c r="D172" t="s">
+        <v>1328</v>
       </c>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
@@ -26377,10 +26422,13 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>1172</v>
+        <v>29</v>
       </c>
       <c r="C173">
         <v>2</v>
+      </c>
+      <c r="D173" t="s">
+        <v>1328</v>
       </c>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
@@ -26388,10 +26436,13 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>1172</v>
+        <v>29</v>
       </c>
       <c r="C174">
         <v>2</v>
+      </c>
+      <c r="D174" t="s">
+        <v>1328</v>
       </c>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
@@ -26399,10 +26450,13 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>1172</v>
+        <v>29</v>
       </c>
       <c r="C175">
         <v>2</v>
+      </c>
+      <c r="D175" t="s">
+        <v>1328</v>
       </c>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
@@ -26410,68 +26464,86 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>1172</v>
+        <v>29</v>
       </c>
       <c r="C176">
         <v>2</v>
       </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D176" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>1172</v>
+        <v>29</v>
       </c>
       <c r="C177">
         <v>2</v>
       </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D177" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>1172</v>
+        <v>29</v>
       </c>
       <c r="C178">
         <v>2</v>
       </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D178" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>1172</v>
+        <v>29</v>
       </c>
       <c r="C179">
         <v>2</v>
       </c>
-    </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D179" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>1172</v>
+        <v>29</v>
       </c>
       <c r="C180">
         <v>2</v>
       </c>
-    </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D180" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>1172</v>
+        <v>29</v>
       </c>
       <c r="C181">
         <v>2</v>
       </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D181" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>181</v>
       </c>
@@ -26481,8 +26553,11 @@
       <c r="C182">
         <v>3</v>
       </c>
-    </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D182" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>182</v>
       </c>
@@ -26492,8 +26567,11 @@
       <c r="C183">
         <v>3</v>
       </c>
-    </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D183" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>183</v>
       </c>
@@ -26503,8 +26581,11 @@
       <c r="C184">
         <v>3</v>
       </c>
-    </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D184" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>184</v>
       </c>
@@ -26514,8 +26595,11 @@
       <c r="C185">
         <v>3</v>
       </c>
-    </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D185" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>185</v>
       </c>
@@ -26525,8 +26609,11 @@
       <c r="C186">
         <v>3</v>
       </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D186" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>186</v>
       </c>
@@ -26536,8 +26623,11 @@
       <c r="C187">
         <v>3</v>
       </c>
-    </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D187" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>187</v>
       </c>
@@ -26547,8 +26637,11 @@
       <c r="C188">
         <v>3</v>
       </c>
-    </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D188" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>188</v>
       </c>
@@ -26558,8 +26651,11 @@
       <c r="C189">
         <v>3</v>
       </c>
-    </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D189" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>189</v>
       </c>
@@ -26569,8 +26665,11 @@
       <c r="C190">
         <v>3</v>
       </c>
-    </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D190" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>190</v>
       </c>
@@ -26580,8 +26679,11 @@
       <c r="C191">
         <v>3</v>
       </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D191" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>191</v>
       </c>
@@ -26591,8 +26693,11 @@
       <c r="C192">
         <v>3</v>
       </c>
-    </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D192" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>192</v>
       </c>
@@ -26602,8 +26707,11 @@
       <c r="C193">
         <v>3</v>
       </c>
-    </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D193" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>193</v>
       </c>
@@ -26613,8 +26721,11 @@
       <c r="C194">
         <v>3</v>
       </c>
-    </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D194" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>194</v>
       </c>
@@ -26624,8 +26735,11 @@
       <c r="C195">
         <v>3</v>
       </c>
-    </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D195" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>195</v>
       </c>
@@ -26635,8 +26749,11 @@
       <c r="C196">
         <v>3</v>
       </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D196" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>196</v>
       </c>
@@ -26646,8 +26763,11 @@
       <c r="C197">
         <v>3</v>
       </c>
-    </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D197" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>197</v>
       </c>
@@ -26657,8 +26777,11 @@
       <c r="C198">
         <v>3</v>
       </c>
-    </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D198" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>198</v>
       </c>
@@ -26668,8 +26791,11 @@
       <c r="C199">
         <v>3</v>
       </c>
-    </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D199" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>199</v>
       </c>
@@ -26679,8 +26805,11 @@
       <c r="C200">
         <v>3</v>
       </c>
-    </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D200" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>200</v>
       </c>
@@ -26690,8 +26819,11 @@
       <c r="C201">
         <v>3</v>
       </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D201" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>201</v>
       </c>
@@ -26701,8 +26833,11 @@
       <c r="C202">
         <v>3</v>
       </c>
-    </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D202" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>202</v>
       </c>
@@ -26712,8 +26847,11 @@
       <c r="C203">
         <v>3</v>
       </c>
-    </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D203" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>203</v>
       </c>
@@ -26723,8 +26861,11 @@
       <c r="C204">
         <v>3</v>
       </c>
-    </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D204" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>204</v>
       </c>
@@ -26734,8 +26875,11 @@
       <c r="C205">
         <v>3</v>
       </c>
-    </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D205" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>205</v>
       </c>
@@ -26745,8 +26889,11 @@
       <c r="C206">
         <v>3</v>
       </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D206" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>206</v>
       </c>
@@ -26756,8 +26903,11 @@
       <c r="C207">
         <v>3</v>
       </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D207" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>207</v>
       </c>
@@ -26767,8 +26917,11 @@
       <c r="C208">
         <v>3</v>
       </c>
-    </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D208" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>208</v>
       </c>
@@ -26778,8 +26931,11 @@
       <c r="C209">
         <v>3</v>
       </c>
-    </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D209" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>209</v>
       </c>
@@ -26789,8 +26945,11 @@
       <c r="C210">
         <v>3</v>
       </c>
-    </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D210" t="s">
+        <v>1328</v>
+      </c>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>210</v>
       </c>
@@ -26799,6 +26958,9 @@
       </c>
       <c r="C211">
         <v>3</v>
+      </c>
+      <c r="D211" t="s">
+        <v>1328</v>
       </c>
     </row>
   </sheetData>
@@ -26810,10 +26972,10 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63F261A1-0426-462C-979C-1324696FD2FB}">
   <sheetPr codeName="Sheet4"/>
-  <dimension ref="A1:O766"/>
+  <dimension ref="A1:O767"/>
   <sheetViews>
-    <sheetView topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="E100" sqref="E100:M104"/>
+    <sheetView tabSelected="1" topLeftCell="A697" workbookViewId="0">
+      <selection activeCell="K711" sqref="K711"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31669,7 +31831,7 @@
         <v>6</v>
       </c>
       <c r="D247">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E247" t="s">
         <v>137</v>
@@ -31757,7 +31919,7 @@
         <v>6</v>
       </c>
       <c r="D252">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E252" t="s">
         <v>137</v>
@@ -39302,6 +39464,9 @@
       <c r="H713" t="s">
         <v>802</v>
       </c>
+      <c r="I713" t="s">
+        <v>797</v>
+      </c>
     </row>
     <row r="714" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E714" t="s">
@@ -39458,6 +39623,9 @@
       <c r="H722" t="s">
         <v>802</v>
       </c>
+      <c r="I722" t="s">
+        <v>797</v>
+      </c>
     </row>
     <row r="723" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E723" t="s">
@@ -39614,6 +39782,9 @@
       <c r="H731" t="s">
         <v>802</v>
       </c>
+      <c r="I731" t="s">
+        <v>797</v>
+      </c>
     </row>
     <row r="732" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E732" t="s">
@@ -39787,6 +39958,9 @@
       <c r="H741" t="s">
         <v>802</v>
       </c>
+      <c r="I741" t="s">
+        <v>797</v>
+      </c>
     </row>
     <row r="742" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E742" t="s">
@@ -39995,6 +40169,9 @@
       <c r="H752" t="s">
         <v>802</v>
       </c>
+      <c r="I752" t="s">
+        <v>797</v>
+      </c>
     </row>
     <row r="753" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E753" t="s">
@@ -40104,71 +40281,47 @@
         <v>11</v>
       </c>
       <c r="E758" t="s">
-        <v>140</v>
-      </c>
-      <c r="F758" t="s">
-        <v>940</v>
-      </c>
-      <c r="G758" t="s">
-        <v>802</v>
-      </c>
-      <c r="H758" t="s">
-        <v>797</v>
+        <v>137</v>
       </c>
     </row>
     <row r="759" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E759" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F759" t="s">
-        <v>141</v>
+        <v>940</v>
       </c>
       <c r="G759" t="s">
-        <v>142</v>
+        <v>802</v>
       </c>
       <c r="H759" t="s">
-        <v>1506</v>
-      </c>
-      <c r="I759" t="s">
-        <v>143</v>
-      </c>
-      <c r="J759" t="s">
-        <v>1507</v>
-      </c>
-      <c r="K759" t="s">
-        <v>144</v>
-      </c>
-      <c r="L759" t="s">
-        <v>802</v>
-      </c>
-      <c r="M759" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="760" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E760" t="s">
-        <v>795</v>
+        <v>139</v>
       </c>
       <c r="F760" t="s">
-        <v>796</v>
+        <v>141</v>
       </c>
       <c r="G760" t="s">
-        <v>1505</v>
+        <v>142</v>
       </c>
       <c r="H760" t="s">
-        <v>264</v>
+        <v>1506</v>
       </c>
       <c r="I760" t="s">
+        <v>143</v>
+      </c>
+      <c r="J760" t="s">
         <v>1507</v>
       </c>
-      <c r="J760" t="s">
+      <c r="K760" t="s">
         <v>144</v>
       </c>
-      <c r="K760" t="s">
-        <v>157</v>
-      </c>
       <c r="L760" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="M760" t="s">
         <v>797</v>
@@ -40176,16 +40329,31 @@
     </row>
     <row r="761" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E761" t="s">
-        <v>139</v>
+        <v>795</v>
       </c>
       <c r="F761" t="s">
-        <v>140</v>
+        <v>796</v>
       </c>
       <c r="G761" t="s">
-        <v>800</v>
+        <v>1505</v>
       </c>
       <c r="H761" t="s">
-        <v>802</v>
+        <v>264</v>
+      </c>
+      <c r="I761" t="s">
+        <v>1507</v>
+      </c>
+      <c r="J761" t="s">
+        <v>144</v>
+      </c>
+      <c r="K761" t="s">
+        <v>157</v>
+      </c>
+      <c r="L761" t="s">
+        <v>804</v>
+      </c>
+      <c r="M761" t="s">
+        <v>797</v>
       </c>
     </row>
     <row r="762" spans="1:14" x14ac:dyDescent="0.25">
@@ -40193,42 +40361,36 @@
         <v>139</v>
       </c>
       <c r="F762" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G762" t="s">
-        <v>142</v>
+        <v>800</v>
       </c>
       <c r="H762" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="I762" t="s">
-        <v>801</v>
-      </c>
-      <c r="J762" t="s">
-        <v>802</v>
-      </c>
-      <c r="K762" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="763" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E763" t="s">
-        <v>940</v>
+        <v>139</v>
       </c>
       <c r="F763" t="s">
-        <v>1502</v>
+        <v>141</v>
       </c>
       <c r="G763" t="s">
-        <v>240</v>
+        <v>142</v>
       </c>
       <c r="H763" t="s">
-        <v>712</v>
+        <v>800</v>
       </c>
       <c r="I763" t="s">
-        <v>956</v>
+        <v>801</v>
       </c>
       <c r="J763" t="s">
-        <v>157</v>
+        <v>802</v>
       </c>
       <c r="K763" t="s">
         <v>797</v>
@@ -40236,49 +40398,72 @@
     </row>
     <row r="764" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E764" t="s">
-        <v>795</v>
+        <v>940</v>
       </c>
       <c r="F764" t="s">
-        <v>796</v>
+        <v>1502</v>
       </c>
       <c r="G764" t="s">
-        <v>1502</v>
+        <v>240</v>
       </c>
       <c r="H764" t="s">
-        <v>817</v>
+        <v>712</v>
       </c>
       <c r="I764" t="s">
-        <v>1481</v>
+        <v>956</v>
       </c>
       <c r="J764" t="s">
-        <v>796</v>
+        <v>157</v>
       </c>
       <c r="K764" t="s">
-        <v>1345</v>
-      </c>
-      <c r="L764" t="s">
-        <v>144</v>
-      </c>
-      <c r="M764" t="s">
-        <v>157</v>
-      </c>
-      <c r="N764" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="765" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E765" t="s">
-        <v>804</v>
+        <v>795</v>
       </c>
       <c r="F765" t="s">
-        <v>804</v>
+        <v>796</v>
       </c>
       <c r="G765" t="s">
+        <v>1502</v>
+      </c>
+      <c r="H765" t="s">
+        <v>817</v>
+      </c>
+      <c r="I765" t="s">
+        <v>1481</v>
+      </c>
+      <c r="J765" t="s">
+        <v>796</v>
+      </c>
+      <c r="K765" t="s">
+        <v>1345</v>
+      </c>
+      <c r="L765" t="s">
+        <v>144</v>
+      </c>
+      <c r="M765" t="s">
+        <v>157</v>
+      </c>
+      <c r="N765" t="s">
         <v>797</v>
       </c>
     </row>
     <row r="766" spans="1:14" x14ac:dyDescent="0.25">
       <c r="E766" t="s">
+        <v>804</v>
+      </c>
+      <c r="F766" t="s">
+        <v>804</v>
+      </c>
+      <c r="G766" t="s">
+        <v>797</v>
+      </c>
+    </row>
+    <row r="767" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E767" t="s">
         <v>138</v>
       </c>
     </row>
@@ -40293,7 +40478,7 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:D201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" workbookViewId="0">
+    <sheetView topLeftCell="A181" workbookViewId="0">
       <selection activeCell="C194" sqref="C194"/>
     </sheetView>
   </sheetViews>
@@ -42417,9 +42602,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -42569,26 +42757,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DC388A3-3E8E-468D-B938-40CD1FB812C5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4344FF14-EBFA-4C51-8BB6-D67423FD69A5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="915c154c-1470-46a8-b038-1496da6ff25f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -42612,9 +42789,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4344FF14-EBFA-4C51-8BB6-D67423FD69A5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DC388A3-3E8E-468D-B938-40CD1FB812C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="915c154c-1470-46a8-b038-1496da6ff25f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fill in the block bug fix
</commit_message>
<xml_diff>
--- a/assets/excel/Minigames.xlsx
+++ b/assets/excel/Minigames.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OEM\Documents\GitHub\CodexLearning\assets\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Ryoshu\Documents\GitHub\CodexLearning2\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F23C315-5E22-4306-9D33-97A37C4245CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07C3917D-DF71-499B-9480-E8FDC2CEC89A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2F4D6A40-7D2F-4386-B1F7-728101A5D7AD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2F4D6A40-7D2F-4386-B1F7-728101A5D7AD}"/>
   </bookViews>
   <sheets>
     <sheet name="CodeRiddle" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Minigame" sheetId="7" r:id="rId3"/>
     <sheet name="AnswerPool2" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,12 +26,8 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10012" uniqueCount="1659">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10009" uniqueCount="1660">
   <si>
     <t>Stage 1</t>
   </si>
@@ -6139,6 +6135,9 @@
   </si>
   <si>
     <t>a=b</t>
+  </si>
+  <si>
+    <t>'A'</t>
   </si>
 </sst>
 </file>
@@ -6596,7 +6595,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:R336"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A268" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A283" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H284" sqref="H284"/>
     </sheetView>
   </sheetViews>
@@ -28700,8 +28699,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:O748"/>
   <sheetViews>
-    <sheetView topLeftCell="A432" workbookViewId="0">
-      <selection activeCell="E479" sqref="E479"/>
+    <sheetView tabSelected="1" topLeftCell="A271" workbookViewId="0">
+      <selection activeCell="G294" sqref="G294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34251,7 +34250,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="289" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E289" t="s">
         <v>181</v>
       </c>
@@ -34271,7 +34270,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="290" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E290" t="s">
         <v>265</v>
       </c>
@@ -34285,7 +34284,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="291" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E291" t="s">
         <v>721</v>
       </c>
@@ -34299,7 +34298,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="292" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E292" t="s">
         <v>728</v>
       </c>
@@ -34313,7 +34312,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="293" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E293" t="s">
         <v>721</v>
       </c>
@@ -34327,7 +34326,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="294" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E294" t="s">
         <v>728</v>
       </c>
@@ -34335,15 +34334,15 @@
         <v>728</v>
       </c>
       <c r="G294" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="295" spans="1:13" x14ac:dyDescent="0.25">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="295" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E295" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="296" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>44</v>
       </c>
@@ -34360,7 +34359,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="297" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E297" t="s">
         <v>136</v>
       </c>
@@ -34383,7 +34382,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="298" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E298" t="s">
         <v>181</v>
       </c>
@@ -34403,7 +34402,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="299" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E299" t="s">
         <v>265</v>
       </c>
@@ -34417,7 +34416,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="300" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E300" t="s">
         <v>721</v>
       </c>
@@ -34431,7 +34430,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="301" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E301" t="s">
         <v>728</v>
       </c>
@@ -34445,7 +34444,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="302" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E302" t="s">
         <v>721</v>
       </c>
@@ -34459,7 +34458,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="303" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E303" t="s">
         <v>728</v>
       </c>
@@ -34467,19 +34466,10 @@
         <v>728</v>
       </c>
       <c r="G303" t="s">
-        <v>151</v>
-      </c>
-      <c r="K303" t="s">
-        <v>151</v>
-      </c>
-      <c r="L303" t="s">
-        <v>728</v>
-      </c>
-      <c r="M303" t="s">
-        <v>723</v>
-      </c>
-    </row>
-    <row r="304" spans="1:13" x14ac:dyDescent="0.25">
+        <v>723</v>
+      </c>
+    </row>
+    <row r="304" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E304" t="s">
         <v>135</v>
       </c>
@@ -35264,7 +35254,7 @@
         <v>225</v>
       </c>
       <c r="H349" s="2" t="s">
-        <v>814</v>
+        <v>1659</v>
       </c>
       <c r="I349" t="s">
         <v>151</v>
@@ -35292,7 +35282,7 @@
         <v>891</v>
       </c>
       <c r="F351" s="2" t="s">
-        <v>814</v>
+        <v>1659</v>
       </c>
       <c r="G351" t="s">
         <v>751</v>
@@ -49270,9 +49260,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -49422,26 +49415,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DC388A3-3E8E-468D-B938-40CD1FB812C5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4344FF14-EBFA-4C51-8BB6-D67423FD69A5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="915c154c-1470-46a8-b038-1496da6ff25f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -49465,9 +49447,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4344FF14-EBFA-4C51-8BB6-D67423FD69A5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0DC388A3-3E8E-468D-B938-40CD1FB812C5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="915c154c-1470-46a8-b038-1496da6ff25f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>